<commit_message>
Started Adding Superstition Info
</commit_message>
<xml_diff>
--- a/Data/Trail Mapping Info.xlsx
+++ b/Data/Trail Mapping Info.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9859" uniqueCount="3495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10096" uniqueCount="3598">
   <si>
     <t>trackID</t>
   </si>
@@ -10506,6 +10506,315 @@
   </si>
   <si>
     <t>Iron River Area</t>
+  </si>
+  <si>
+    <t>Superstition Wilderness</t>
+  </si>
+  <si>
+    <t>WVCV01</t>
+  </si>
+  <si>
+    <t>arrive Wave Cave</t>
+  </si>
+  <si>
+    <t>WVCV02</t>
+  </si>
+  <si>
+    <t>WVCV03</t>
+  </si>
+  <si>
+    <t>WVCV04</t>
+  </si>
+  <si>
+    <t>PFMT01</t>
+  </si>
+  <si>
+    <t>arrive Fremont Saddle</t>
+  </si>
+  <si>
+    <t>PNNT01</t>
+  </si>
+  <si>
+    <t>Fremont Saddle to Weaver's Needle Pinion Tree</t>
+  </si>
+  <si>
+    <t>leave Fremont Saddle</t>
+  </si>
+  <si>
+    <t>arrive Pinion Tree</t>
+  </si>
+  <si>
+    <t>CVFS01</t>
+  </si>
+  <si>
+    <t>leave Peralta Tr (102)</t>
+  </si>
+  <si>
+    <t>Dacite Cliff Mine Tr</t>
+  </si>
+  <si>
+    <t>CVFS02</t>
+  </si>
+  <si>
+    <t>merge Bluff Spring Tr (235)</t>
+  </si>
+  <si>
+    <t>CVFS03</t>
+  </si>
+  <si>
+    <t>CVFS04</t>
+  </si>
+  <si>
+    <t>arrive Peralta TH</t>
+  </si>
+  <si>
+    <t>MSCR01</t>
+  </si>
+  <si>
+    <t>MSCR02</t>
+  </si>
+  <si>
+    <t>MSCR03</t>
+  </si>
+  <si>
+    <t>Massacre Grounds Tr</t>
+  </si>
+  <si>
+    <t>Massacre Grounds Tr (Waterfall spur)</t>
+  </si>
+  <si>
+    <t>Massacre Grounds Peak</t>
+  </si>
+  <si>
+    <t>Massacre Grounds Waterfall</t>
+  </si>
+  <si>
+    <t>MSCR02, MSCR03</t>
+  </si>
+  <si>
+    <t>MSCR01, MSCR03</t>
+  </si>
+  <si>
+    <t>HGPH01</t>
+  </si>
+  <si>
+    <t>Heiroglyphics Tr</t>
+  </si>
+  <si>
+    <t>Crosscut TH parking</t>
+  </si>
+  <si>
+    <t>Heiroglphics TH parking</t>
+  </si>
+  <si>
+    <t>Peralto Tr (102) to Fremont Saddle</t>
+  </si>
+  <si>
+    <t>leave Peralta TH parking</t>
+  </si>
+  <si>
+    <t>Carney Springs TH parking</t>
+  </si>
+  <si>
+    <t>Cave Trail Hike (across Fremont Saddle)</t>
+  </si>
+  <si>
+    <t>Cave Trail Hike (Bluff Spring Tr)</t>
+  </si>
+  <si>
+    <t>Cave Trail Hike (Dutchman's Tr)</t>
+  </si>
+  <si>
+    <t>Wave Cave Hike (Lost Goldmine Tr East)</t>
+  </si>
+  <si>
+    <t>Lost Goldmine Tr East</t>
+  </si>
+  <si>
+    <t>Heiroglyphics Canyon</t>
+  </si>
+  <si>
+    <t>HGPH02</t>
+  </si>
+  <si>
+    <t>BMSA01</t>
+  </si>
+  <si>
+    <t>Black Mesa Hike (Dutchman's Tr 104)</t>
+  </si>
+  <si>
+    <t>First Water TH parking</t>
+  </si>
+  <si>
+    <t>Second Water Tr (236)</t>
+  </si>
+  <si>
+    <t>Tim's Saddle Tr</t>
+  </si>
+  <si>
+    <t>W Boulder Canyon Tr</t>
+  </si>
+  <si>
+    <t>Boulder Canyon Tr (103)</t>
+  </si>
+  <si>
+    <t>BMSA02</t>
+  </si>
+  <si>
+    <t>BMSA03</t>
+  </si>
+  <si>
+    <t>BMSA04</t>
+  </si>
+  <si>
+    <t>BMSA05</t>
+  </si>
+  <si>
+    <t>BMSA06</t>
+  </si>
+  <si>
+    <t>BMSA07</t>
+  </si>
+  <si>
+    <t>Black Mesa Hike (Bull Pass Tr 129)</t>
+  </si>
+  <si>
+    <t>leave Dutchman's Tr / start Bull Pass Tr</t>
+  </si>
+  <si>
+    <t>Black Top Mesa</t>
+  </si>
+  <si>
+    <t>BMSA08</t>
+  </si>
+  <si>
+    <t>BMSA10</t>
+  </si>
+  <si>
+    <t>Black Mesa Hike (Black Mesa Tr 241)</t>
+  </si>
+  <si>
+    <t>Black Mesa Tr (241)</t>
+  </si>
+  <si>
+    <t>leave Dutchman's Tr / start Black Mesa Tr</t>
+  </si>
+  <si>
+    <t>BMSA04, BMSA05</t>
+  </si>
+  <si>
+    <t>BMSA06, BMSA10</t>
+  </si>
+  <si>
+    <t>BMSA05, BMSA10</t>
+  </si>
+  <si>
+    <t>leave Black Mesa Tr / start Second Water Tr</t>
+  </si>
+  <si>
+    <t>Black Mesa Hike (Second Water Tr 236)</t>
+  </si>
+  <si>
+    <t>BMSA11</t>
+  </si>
+  <si>
+    <t>Hackberry Springs Tr [South]</t>
+  </si>
+  <si>
+    <t>Hackberry Springs Tr [North]</t>
+  </si>
+  <si>
+    <t>Dutchman's Tr (104)</t>
+  </si>
+  <si>
+    <t>BMSA12</t>
+  </si>
+  <si>
+    <t>BMSA13</t>
+  </si>
+  <si>
+    <t>BMSA01, BMSA02</t>
+  </si>
+  <si>
+    <t>BMSA02, BMSA13</t>
+  </si>
+  <si>
+    <t>BMSA01, BMSA13</t>
+  </si>
+  <si>
+    <t>Black Mesa Hike (Black Top Mesa Tr)</t>
+  </si>
+  <si>
+    <t>leave Bull Pass Tr / start Black Top Mesa Tr</t>
+  </si>
+  <si>
+    <t>leave Bull Pass Tr / Black Top Mesa Tr</t>
+  </si>
+  <si>
+    <t>Wave Cave Hike (Carney Springs Tr)</t>
+  </si>
+  <si>
+    <t>merge Carney Springs Tr</t>
+  </si>
+  <si>
+    <t>leave Carney Springs Tr / start Wave Cave Tr</t>
+  </si>
+  <si>
+    <t>Wave Cave Hike (Wave Cave Tr)</t>
+  </si>
+  <si>
+    <t>Cave Trail Hike (Cave TR)</t>
+  </si>
+  <si>
+    <t>merge Dutchman's Tr (104)</t>
+  </si>
+  <si>
+    <t>IMG_0438</t>
+  </si>
+  <si>
+    <t>IMG_0441</t>
+  </si>
+  <si>
+    <t>IMG_0444</t>
+  </si>
+  <si>
+    <t>IMG_0446</t>
+  </si>
+  <si>
+    <t>IMG_0448</t>
+  </si>
+  <si>
+    <t>IMG_0451</t>
+  </si>
+  <si>
+    <t>IMG_0455</t>
+  </si>
+  <si>
+    <t>IMG_0461</t>
+  </si>
+  <si>
+    <t>IMG_0463</t>
+  </si>
+  <si>
+    <t>IMG_0468</t>
+  </si>
+  <si>
+    <t>Kim with a Saguaro</t>
+  </si>
+  <si>
+    <t>Typical scenery in Spring 2022</t>
+  </si>
+  <si>
+    <t>Kim climbing to the Wave Cave</t>
+  </si>
+  <si>
+    <t>Us at the Wave Cave</t>
+  </si>
+  <si>
+    <t>Wave Cave</t>
+  </si>
+  <si>
+    <t>Looking back to the Wave Cave</t>
   </si>
 </sst>
 </file>
@@ -10854,13 +11163,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X1002"/>
+  <dimension ref="A1:X1028"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B992" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:A2"/>
+      <selection pane="bottomRight" activeCell="G1004" sqref="G1004"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37780,7 +38089,732 @@
       </c>
     </row>
     <row r="1002" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1002" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1002" s="3" t="s">
+        <v>3496</v>
+      </c>
+      <c r="C1002" s="3" t="s">
+        <v>3534</v>
+      </c>
+      <c r="D1002">
+        <v>2022</v>
+      </c>
+      <c r="E1002" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1002" s="3" t="s">
+        <v>3530</v>
+      </c>
+      <c r="G1002" s="3" t="s">
+        <v>3509</v>
+      </c>
       <c r="H1002" s="3"/>
+      <c r="I1002" s="3" t="s">
+        <v>3498</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1003" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1003" s="3" t="s">
+        <v>3498</v>
+      </c>
+      <c r="C1003" s="3" t="s">
+        <v>3534</v>
+      </c>
+      <c r="D1003">
+        <v>2022</v>
+      </c>
+      <c r="E1003" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1003" s="3" t="s">
+        <v>3509</v>
+      </c>
+      <c r="G1003" s="3" t="s">
+        <v>3577</v>
+      </c>
+      <c r="H1003" s="3" t="s">
+        <v>3496</v>
+      </c>
+      <c r="I1003" s="3" t="s">
+        <v>3499</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1004" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1004" s="3" t="s">
+        <v>3499</v>
+      </c>
+      <c r="C1004" s="3" t="s">
+        <v>3576</v>
+      </c>
+      <c r="D1004">
+        <v>2022</v>
+      </c>
+      <c r="E1004" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1004" s="3" t="s">
+        <v>3577</v>
+      </c>
+      <c r="G1004" s="3" t="s">
+        <v>3578</v>
+      </c>
+      <c r="H1004" s="3" t="s">
+        <v>3498</v>
+      </c>
+      <c r="I1004" s="3" t="s">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1005" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1005" s="3" t="s">
+        <v>3500</v>
+      </c>
+      <c r="C1005" s="3" t="s">
+        <v>3579</v>
+      </c>
+      <c r="D1005">
+        <v>2022</v>
+      </c>
+      <c r="E1005" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1005" s="3" t="s">
+        <v>3578</v>
+      </c>
+      <c r="G1005" s="3" t="s">
+        <v>3497</v>
+      </c>
+      <c r="H1005" s="3" t="s">
+        <v>3499</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1006" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1006" s="3" t="s">
+        <v>3501</v>
+      </c>
+      <c r="C1006" s="3" t="s">
+        <v>3528</v>
+      </c>
+      <c r="D1006">
+        <v>2022</v>
+      </c>
+      <c r="E1006" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1006" s="3" t="s">
+        <v>3529</v>
+      </c>
+      <c r="G1006" s="3" t="s">
+        <v>3502</v>
+      </c>
+      <c r="I1006" s="3" t="s">
+        <v>3503</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1007" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1007" s="3" t="s">
+        <v>3503</v>
+      </c>
+      <c r="C1007" s="3" t="s">
+        <v>3504</v>
+      </c>
+      <c r="D1007">
+        <v>2022</v>
+      </c>
+      <c r="E1007" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1007" s="3" t="s">
+        <v>3505</v>
+      </c>
+      <c r="G1007" s="3" t="s">
+        <v>3506</v>
+      </c>
+      <c r="H1007" s="3" t="s">
+        <v>3501</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1008" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1008" s="3" t="s">
+        <v>3507</v>
+      </c>
+      <c r="C1008" s="3" t="s">
+        <v>3531</v>
+      </c>
+      <c r="D1008">
+        <v>2022</v>
+      </c>
+      <c r="E1008" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1008" s="3" t="s">
+        <v>3508</v>
+      </c>
+      <c r="G1008" s="3" t="s">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1009" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1009" s="3" t="s">
+        <v>3510</v>
+      </c>
+      <c r="C1009" s="3" t="s">
+        <v>3580</v>
+      </c>
+      <c r="D1009">
+        <v>2022</v>
+      </c>
+      <c r="E1009" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1009" s="3" t="s">
+        <v>3505</v>
+      </c>
+      <c r="G1009" s="3" t="s">
+        <v>3511</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1010" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1010" s="3" t="s">
+        <v>3512</v>
+      </c>
+      <c r="C1010" s="3" t="s">
+        <v>3532</v>
+      </c>
+      <c r="D1010">
+        <v>2022</v>
+      </c>
+      <c r="E1010" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1010" s="3" t="s">
+        <v>3511</v>
+      </c>
+      <c r="G1010" s="3" t="s">
+        <v>3581</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1011" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1011" s="3" t="s">
+        <v>3513</v>
+      </c>
+      <c r="C1011" s="3" t="s">
+        <v>3533</v>
+      </c>
+      <c r="D1011">
+        <v>2022</v>
+      </c>
+      <c r="E1011" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1011" s="3" t="s">
+        <v>3581</v>
+      </c>
+      <c r="G1011" s="3" t="s">
+        <v>3514</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1012" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1012" s="3" t="s">
+        <v>3515</v>
+      </c>
+      <c r="C1012" s="3" t="s">
+        <v>3518</v>
+      </c>
+      <c r="D1012">
+        <v>2022</v>
+      </c>
+      <c r="E1012" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1012" s="3" t="s">
+        <v>3526</v>
+      </c>
+      <c r="G1012" s="3" t="s">
+        <v>3519</v>
+      </c>
+      <c r="I1012" s="3" t="s">
+        <v>3522</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1013" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1013" s="3" t="s">
+        <v>3516</v>
+      </c>
+      <c r="C1013" s="3" t="s">
+        <v>3518</v>
+      </c>
+      <c r="D1013">
+        <v>2022</v>
+      </c>
+      <c r="E1013" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1013" s="3" t="s">
+        <v>3519</v>
+      </c>
+      <c r="G1013" s="3" t="s">
+        <v>3520</v>
+      </c>
+      <c r="H1013" s="3" t="s">
+        <v>3523</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1014" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1014" s="3" t="s">
+        <v>3517</v>
+      </c>
+      <c r="C1014" s="3" t="s">
+        <v>3519</v>
+      </c>
+      <c r="D1014">
+        <v>2022</v>
+      </c>
+      <c r="E1014" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1014" s="3" t="s">
+        <v>3518</v>
+      </c>
+      <c r="G1014" s="3" t="s">
+        <v>3521</v>
+      </c>
+      <c r="H1014" s="3" t="s">
+        <v>3522</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1015" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1015" s="3" t="s">
+        <v>3524</v>
+      </c>
+      <c r="C1015" s="3" t="s">
+        <v>3525</v>
+      </c>
+      <c r="D1015">
+        <v>2022</v>
+      </c>
+      <c r="E1015" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1015" s="3" t="s">
+        <v>3527</v>
+      </c>
+      <c r="G1015" s="3" t="s">
+        <v>3535</v>
+      </c>
+      <c r="I1015" s="3" t="s">
+        <v>3537</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1016" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1016" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C1016" s="3" t="s">
+        <v>3525</v>
+      </c>
+      <c r="D1016">
+        <v>2022</v>
+      </c>
+      <c r="E1016" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1016" s="3" t="s">
+        <v>3535</v>
+      </c>
+      <c r="G1016" s="3" t="s">
+        <v>3536</v>
+      </c>
+      <c r="H1016" s="3" t="s">
+        <v>3524</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1017" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1017" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="C1017" s="3" t="s">
+        <v>3539</v>
+      </c>
+      <c r="D1017">
+        <v>2022</v>
+      </c>
+      <c r="E1017" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1017" s="3" t="s">
+        <v>3540</v>
+      </c>
+      <c r="G1017" s="3" t="s">
+        <v>3541</v>
+      </c>
+      <c r="I1017" s="3" t="s">
+        <v>3571</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1018" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1018" s="3" t="s">
+        <v>3545</v>
+      </c>
+      <c r="C1018" s="3" t="s">
+        <v>3539</v>
+      </c>
+      <c r="D1018">
+        <v>2022</v>
+      </c>
+      <c r="E1018" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1018" s="3" t="s">
+        <v>3541</v>
+      </c>
+      <c r="G1018" s="3" t="s">
+        <v>3542</v>
+      </c>
+      <c r="H1018" s="3" t="s">
+        <v>3572</v>
+      </c>
+      <c r="I1018" s="3" t="s">
+        <v>3546</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1019" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1019" s="3" t="s">
+        <v>3546</v>
+      </c>
+      <c r="C1019" s="3" t="s">
+        <v>3539</v>
+      </c>
+      <c r="D1019">
+        <v>2022</v>
+      </c>
+      <c r="E1019" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1019" s="3" t="s">
+        <v>3542</v>
+      </c>
+      <c r="G1019" s="3" t="s">
+        <v>3543</v>
+      </c>
+      <c r="H1019" s="3" t="s">
+        <v>3545</v>
+      </c>
+      <c r="I1019" s="3" t="s">
+        <v>3547</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1020" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1020" s="3" t="s">
+        <v>3547</v>
+      </c>
+      <c r="C1020" s="3" t="s">
+        <v>3539</v>
+      </c>
+      <c r="D1020">
+        <v>2022</v>
+      </c>
+      <c r="E1020" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1020" s="3" t="s">
+        <v>3543</v>
+      </c>
+      <c r="G1020" s="3" t="s">
+        <v>3557</v>
+      </c>
+      <c r="H1020" s="3" t="s">
+        <v>3546</v>
+      </c>
+      <c r="I1020" s="3" t="s">
+        <v>3548</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1021" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1021" s="3" t="s">
+        <v>3548</v>
+      </c>
+      <c r="C1021" s="3" t="s">
+        <v>3539</v>
+      </c>
+      <c r="D1021">
+        <v>2022</v>
+      </c>
+      <c r="E1021" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1021" s="3" t="s">
+        <v>3557</v>
+      </c>
+      <c r="G1021" s="3" t="s">
+        <v>3544</v>
+      </c>
+      <c r="H1021" s="3" t="s">
+        <v>3547</v>
+      </c>
+      <c r="I1021" s="3" t="s">
+        <v>3560</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1022" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1022" s="3" t="s">
+        <v>3549</v>
+      </c>
+      <c r="C1022" s="3" t="s">
+        <v>3539</v>
+      </c>
+      <c r="D1022">
+        <v>2022</v>
+      </c>
+      <c r="E1022" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1022" s="3" t="s">
+        <v>3544</v>
+      </c>
+      <c r="G1022" s="3" t="s">
+        <v>3552</v>
+      </c>
+      <c r="H1022" s="3" t="s">
+        <v>3561</v>
+      </c>
+      <c r="I1022" s="3" t="s">
+        <v>3550</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1023" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1023" s="3" t="s">
+        <v>3550</v>
+      </c>
+      <c r="C1023" s="3" t="s">
+        <v>3551</v>
+      </c>
+      <c r="D1023">
+        <v>2022</v>
+      </c>
+      <c r="E1023" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1023" s="3" t="s">
+        <v>3552</v>
+      </c>
+      <c r="G1023" s="3" t="s">
+        <v>3575</v>
+      </c>
+      <c r="H1023" s="3" t="s">
+        <v>3549</v>
+      </c>
+      <c r="I1023" s="3" t="s">
+        <v>3554</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1024" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1024" s="3" t="s">
+        <v>3554</v>
+      </c>
+      <c r="C1024" s="3" t="s">
+        <v>3573</v>
+      </c>
+      <c r="D1024">
+        <v>2022</v>
+      </c>
+      <c r="E1024" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1024" s="3" t="s">
+        <v>3574</v>
+      </c>
+      <c r="G1024" s="3" t="s">
+        <v>3553</v>
+      </c>
+      <c r="H1024" s="3" t="s">
+        <v>3550</v>
+      </c>
+      <c r="I1024" s="3"/>
+    </row>
+    <row r="1025" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1025" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1025" s="3" t="s">
+        <v>3555</v>
+      </c>
+      <c r="C1025" s="3" t="s">
+        <v>3556</v>
+      </c>
+      <c r="D1025">
+        <v>2022</v>
+      </c>
+      <c r="E1025" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1025" s="3" t="s">
+        <v>3558</v>
+      </c>
+      <c r="G1025" s="3" t="s">
+        <v>3562</v>
+      </c>
+      <c r="H1025" s="3" t="s">
+        <v>3559</v>
+      </c>
+      <c r="I1025" s="3" t="s">
+        <v>3564</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1026" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1026" s="3" t="s">
+        <v>3564</v>
+      </c>
+      <c r="C1026" s="3" t="s">
+        <v>3563</v>
+      </c>
+      <c r="D1026">
+        <v>2022</v>
+      </c>
+      <c r="E1026" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1026" s="3" t="s">
+        <v>3562</v>
+      </c>
+      <c r="G1026" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="H1026" s="3" t="s">
+        <v>3555</v>
+      </c>
+      <c r="I1026" s="3" t="s">
+        <v>3568</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1027" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1027" s="3" t="s">
+        <v>3568</v>
+      </c>
+      <c r="C1027" s="3" t="s">
+        <v>3563</v>
+      </c>
+      <c r="D1027">
+        <v>2022</v>
+      </c>
+      <c r="E1027" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1027" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="G1027" s="3" t="s">
+        <v>3565</v>
+      </c>
+      <c r="H1027" s="3" t="s">
+        <v>3564</v>
+      </c>
+      <c r="I1027" s="3" t="s">
+        <v>3569</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1028" s="3" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B1028" s="3" t="s">
+        <v>3569</v>
+      </c>
+      <c r="C1028" s="3" t="s">
+        <v>3563</v>
+      </c>
+      <c r="D1028">
+        <v>2022</v>
+      </c>
+      <c r="E1028" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1028" s="3" t="s">
+        <v>3565</v>
+      </c>
+      <c r="G1028" s="3" t="s">
+        <v>3567</v>
+      </c>
+      <c r="H1028" s="3" t="s">
+        <v>3568</v>
+      </c>
+      <c r="I1028" s="3" t="s">
+        <v>3570</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -64114,16 +65148,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z411"/>
+  <dimension ref="A1:Z421"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A397" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A422" sqref="A422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.44140625" bestFit="1" customWidth="1"/>
@@ -69921,6 +70955,146 @@
         <v>3138</v>
       </c>
     </row>
+    <row r="412" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A412" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B412" t="s">
+        <v>3496</v>
+      </c>
+      <c r="C412" s="16" t="s">
+        <v>3582</v>
+      </c>
+      <c r="D412" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A413" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B413" t="s">
+        <v>3496</v>
+      </c>
+      <c r="C413" s="16" t="s">
+        <v>3583</v>
+      </c>
+      <c r="D413" t="s">
+        <v>3593</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A414" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B414" t="s">
+        <v>3499</v>
+      </c>
+      <c r="C414" s="16" t="s">
+        <v>3584</v>
+      </c>
+      <c r="D414" t="s">
+        <v>3593</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A415" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B415" t="s">
+        <v>3500</v>
+      </c>
+      <c r="C415" s="16" t="s">
+        <v>3585</v>
+      </c>
+      <c r="D415" t="s">
+        <v>3594</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A416" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B416" t="s">
+        <v>3500</v>
+      </c>
+      <c r="C416" s="16" t="s">
+        <v>3586</v>
+      </c>
+      <c r="D416" t="s">
+        <v>3594</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A417" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B417" t="s">
+        <v>3500</v>
+      </c>
+      <c r="C417" s="16" t="s">
+        <v>3587</v>
+      </c>
+      <c r="D417" t="s">
+        <v>3595</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A418" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B418" t="s">
+        <v>3500</v>
+      </c>
+      <c r="C418" s="16" t="s">
+        <v>3588</v>
+      </c>
+      <c r="D418" t="s">
+        <v>3596</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A419" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B419" t="s">
+        <v>3500</v>
+      </c>
+      <c r="C419" s="16" t="s">
+        <v>3589</v>
+      </c>
+      <c r="D419" t="s">
+        <v>3595</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A420" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B420" t="s">
+        <v>3500</v>
+      </c>
+      <c r="C420" s="16" t="s">
+        <v>3590</v>
+      </c>
+      <c r="D420" t="s">
+        <v>3595</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A421" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B421" t="s">
+        <v>3500</v>
+      </c>
+      <c r="C421" s="16" t="s">
+        <v>3591</v>
+      </c>
+      <c r="D421" t="s">
+        <v>3597</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added more Superstition pictures
</commit_message>
<xml_diff>
--- a/Data/Trail Mapping Info.xlsx
+++ b/Data/Trail Mapping Info.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10096" uniqueCount="3598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10380" uniqueCount="3704">
   <si>
     <t>trackID</t>
   </si>
@@ -10799,9 +10799,6 @@
     <t>IMG_0468</t>
   </si>
   <si>
-    <t>Kim with a Saguaro</t>
-  </si>
-  <si>
     <t>Typical scenery in Spring 2022</t>
   </si>
   <si>
@@ -10815,6 +10812,327 @@
   </si>
   <si>
     <t>Looking back to the Wave Cave</t>
+  </si>
+  <si>
+    <t>IMG_0481</t>
+  </si>
+  <si>
+    <t>IMG_0487</t>
+  </si>
+  <si>
+    <t>IMG_0488</t>
+  </si>
+  <si>
+    <t>IMG_0492</t>
+  </si>
+  <si>
+    <t>IMG_0496</t>
+  </si>
+  <si>
+    <t>IMG_0497</t>
+  </si>
+  <si>
+    <t>IMG_0500</t>
+  </si>
+  <si>
+    <t>IMG_0502</t>
+  </si>
+  <si>
+    <t>IMG_0504</t>
+  </si>
+  <si>
+    <t>IMG_0507</t>
+  </si>
+  <si>
+    <t>IMG_0513</t>
+  </si>
+  <si>
+    <t>IMG_0516</t>
+  </si>
+  <si>
+    <t>IMG_0517</t>
+  </si>
+  <si>
+    <t>IMG_0521</t>
+  </si>
+  <si>
+    <t>IMG_0527</t>
+  </si>
+  <si>
+    <t>IMG_0528</t>
+  </si>
+  <si>
+    <t>IMG_0529</t>
+  </si>
+  <si>
+    <t>Looking further up the canyon</t>
+  </si>
+  <si>
+    <t>Petroglyphs</t>
+  </si>
+  <si>
+    <t>Kim and I in the canyon</t>
+  </si>
+  <si>
+    <t>Ocotillo</t>
+  </si>
+  <si>
+    <t>Blooming Poppy spp.</t>
+  </si>
+  <si>
+    <t>Blooming something(?)</t>
+  </si>
+  <si>
+    <t>Prickly Pear Cactus</t>
+  </si>
+  <si>
+    <t>Saguaro Cactus</t>
+  </si>
+  <si>
+    <t>Old-man Cactus (?)</t>
+  </si>
+  <si>
+    <t>Kim with a Saguaro Cactus</t>
+  </si>
+  <si>
+    <t>IMG_0584</t>
+  </si>
+  <si>
+    <t>IMG_0586</t>
+  </si>
+  <si>
+    <t>IMG_0588</t>
+  </si>
+  <si>
+    <t>IMG_0590</t>
+  </si>
+  <si>
+    <t>IMG_0594</t>
+  </si>
+  <si>
+    <t>IMG_0596</t>
+  </si>
+  <si>
+    <t>IMG_0601</t>
+  </si>
+  <si>
+    <t>IMG_0605</t>
+  </si>
+  <si>
+    <t>IMG_0607</t>
+  </si>
+  <si>
+    <t>IMG_0611</t>
+  </si>
+  <si>
+    <t>IMG_0614</t>
+  </si>
+  <si>
+    <t>IMG_0616</t>
+  </si>
+  <si>
+    <t>IMG_0622</t>
+  </si>
+  <si>
+    <t>IMG_0625</t>
+  </si>
+  <si>
+    <t>IMG_0627</t>
+  </si>
+  <si>
+    <t>IMG_0631</t>
+  </si>
+  <si>
+    <t>IMG_0633</t>
+  </si>
+  <si>
+    <t>Sign near trailhead</t>
+  </si>
+  <si>
+    <t>Kim and I on Fremont Saddle</t>
+  </si>
+  <si>
+    <t>Weaver's Needle from Fremont Saddle</t>
+  </si>
+  <si>
+    <t>Weaver's Needle on way to Pinion tree</t>
+  </si>
+  <si>
+    <t>Pinion tree</t>
+  </si>
+  <si>
+    <t>Kim scrambling</t>
+  </si>
+  <si>
+    <t>Thankful for cairns</t>
+  </si>
+  <si>
+    <t>IMG_0658</t>
+  </si>
+  <si>
+    <t>IMG_0662</t>
+  </si>
+  <si>
+    <t>IMG_0667</t>
+  </si>
+  <si>
+    <t>IMG_0669</t>
+  </si>
+  <si>
+    <t>IMG_0671</t>
+  </si>
+  <si>
+    <t>IMG_0673</t>
+  </si>
+  <si>
+    <t>IMG_0675</t>
+  </si>
+  <si>
+    <t>IMG_0676</t>
+  </si>
+  <si>
+    <t>IMG_0681</t>
+  </si>
+  <si>
+    <t>IMG_0686</t>
+  </si>
+  <si>
+    <t>IMG_0691</t>
+  </si>
+  <si>
+    <t>IMG_0693</t>
+  </si>
+  <si>
+    <t>IMG_0699</t>
+  </si>
+  <si>
+    <t>IMG_0702</t>
+  </si>
+  <si>
+    <t>IMG_0704</t>
+  </si>
+  <si>
+    <t>IMG_0706</t>
+  </si>
+  <si>
+    <t>IMG_0708</t>
+  </si>
+  <si>
+    <t>IMG_0712</t>
+  </si>
+  <si>
+    <t>IMG_0716</t>
+  </si>
+  <si>
+    <t>IMG_0722</t>
+  </si>
+  <si>
+    <t>IMG_0725</t>
+  </si>
+  <si>
+    <t>IMG_0726</t>
+  </si>
+  <si>
+    <t>A reminder</t>
+  </si>
+  <si>
+    <t>Sign to Bull Pass Tr</t>
+  </si>
+  <si>
+    <t>Tiny view of Weaver's Needle</t>
+  </si>
+  <si>
+    <t>Climbing to Black Top Mesa</t>
+  </si>
+  <si>
+    <t>Nearing the top of Black Top Mesa</t>
+  </si>
+  <si>
+    <t>Weaver's Needle from Black Top Mesa</t>
+  </si>
+  <si>
+    <t>Looking back on Black Top Mesa</t>
+  </si>
+  <si>
+    <t>Grazing horses on Black Top Mesa</t>
+  </si>
+  <si>
+    <t>Switching trails for return trip</t>
+  </si>
+  <si>
+    <t>Switching trails on return trip</t>
+  </si>
+  <si>
+    <t>Something blooming</t>
+  </si>
+  <si>
+    <t>Kim with Weaver's Needle</t>
+  </si>
+  <si>
+    <t>IMG_0777</t>
+  </si>
+  <si>
+    <t>IMG_0780</t>
+  </si>
+  <si>
+    <t>IMG_0785</t>
+  </si>
+  <si>
+    <t>IMG_0787</t>
+  </si>
+  <si>
+    <t>IMG_0794</t>
+  </si>
+  <si>
+    <t>IMG_0797</t>
+  </si>
+  <si>
+    <t>IMG_0798</t>
+  </si>
+  <si>
+    <t>IMG_0803</t>
+  </si>
+  <si>
+    <t>IMG_0810</t>
+  </si>
+  <si>
+    <t>IMG_0813</t>
+  </si>
+  <si>
+    <t>IMG_0816</t>
+  </si>
+  <si>
+    <t>IMG_0818</t>
+  </si>
+  <si>
+    <t>IMG_0824</t>
+  </si>
+  <si>
+    <t>IMG_0832</t>
+  </si>
+  <si>
+    <t>IMG_0838</t>
+  </si>
+  <si>
+    <t>Cliff at end of trail</t>
+  </si>
+  <si>
+    <t>Massacre Falls</t>
+  </si>
+  <si>
+    <t>Kim and I at Massacre Falls</t>
+  </si>
+  <si>
+    <t>Me with Prickly Pear Cactus</t>
+  </si>
+  <si>
+    <t>Me with ??? Cactus</t>
+  </si>
+  <si>
+    <t>Me with Ocotilla</t>
+  </si>
+  <si>
+    <t>Kim on the trail</t>
   </si>
 </sst>
 </file>
@@ -11166,10 +11484,10 @@
   <dimension ref="A1:X1028"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B992" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1009" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1004" sqref="G1004"/>
+      <selection pane="bottomRight" activeCell="B1012" sqref="B1012"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -65148,11 +65466,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z421"/>
+  <dimension ref="A1:Z492"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A397" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A422" sqref="A422"/>
+      <pane ySplit="1" topLeftCell="A474" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D487" sqref="D487"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -70966,7 +71284,7 @@
         <v>3582</v>
       </c>
       <c r="D412" t="s">
-        <v>3592</v>
+        <v>3623</v>
       </c>
     </row>
     <row r="413" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -70980,7 +71298,7 @@
         <v>3583</v>
       </c>
       <c r="D413" t="s">
-        <v>3593</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="414" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -70994,7 +71312,7 @@
         <v>3584</v>
       </c>
       <c r="D414" t="s">
-        <v>3593</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="415" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -71008,7 +71326,7 @@
         <v>3585</v>
       </c>
       <c r="D415" t="s">
-        <v>3594</v>
+        <v>3593</v>
       </c>
     </row>
     <row r="416" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -71022,7 +71340,7 @@
         <v>3586</v>
       </c>
       <c r="D416" t="s">
-        <v>3594</v>
+        <v>3593</v>
       </c>
     </row>
     <row r="417" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -71036,7 +71354,7 @@
         <v>3587</v>
       </c>
       <c r="D417" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
     </row>
     <row r="418" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -71050,7 +71368,7 @@
         <v>3588</v>
       </c>
       <c r="D418" t="s">
-        <v>3596</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="419" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -71064,7 +71382,7 @@
         <v>3589</v>
       </c>
       <c r="D419" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
     </row>
     <row r="420" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -71078,7 +71396,7 @@
         <v>3590</v>
       </c>
       <c r="D420" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
     </row>
     <row r="421" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -71092,7 +71410,1001 @@
         <v>3591</v>
       </c>
       <c r="D421" t="s">
+        <v>3596</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A422" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B422" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C422" s="16" t="s">
         <v>3597</v>
+      </c>
+      <c r="D422" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A423" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B423" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C423" s="16" t="s">
+        <v>3598</v>
+      </c>
+      <c r="D423" t="s">
+        <v>3615</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A424" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B424" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C424" s="16" t="s">
+        <v>3599</v>
+      </c>
+      <c r="D424" t="s">
+        <v>3615</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A425" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B425" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C425" s="16" t="s">
+        <v>3600</v>
+      </c>
+      <c r="D425" t="s">
+        <v>3615</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A426" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B426" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C426" s="16" t="s">
+        <v>3601</v>
+      </c>
+      <c r="D426" t="s">
+        <v>3614</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A427" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B427" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C427" s="16" t="s">
+        <v>3602</v>
+      </c>
+      <c r="D427" t="s">
+        <v>3616</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A428" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B428" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C428" s="16" t="s">
+        <v>3603</v>
+      </c>
+      <c r="D428" t="s">
+        <v>3615</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A429" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B429" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C429" s="16" t="s">
+        <v>3604</v>
+      </c>
+      <c r="D429" t="s">
+        <v>3615</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A430" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B430" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C430" s="16" t="s">
+        <v>3605</v>
+      </c>
+      <c r="D430" t="s">
+        <v>3615</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A431" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B431" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C431" s="16" t="s">
+        <v>3606</v>
+      </c>
+      <c r="D431" t="s">
+        <v>3621</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A432" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B432" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C432" s="16" t="s">
+        <v>3607</v>
+      </c>
+      <c r="D432" t="s">
+        <v>3622</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A433" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B433" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C433" s="16" t="s">
+        <v>3608</v>
+      </c>
+      <c r="D433" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A434" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B434" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C434" s="16" t="s">
+        <v>3609</v>
+      </c>
+      <c r="D434" t="s">
+        <v>3619</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A435" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B435" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C435" s="16" t="s">
+        <v>3610</v>
+      </c>
+      <c r="D435" t="s">
+        <v>3617</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A436" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B436" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C436" s="16" t="s">
+        <v>3611</v>
+      </c>
+      <c r="D436" t="s">
+        <v>3620</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A437" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B437" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C437" s="16" t="s">
+        <v>3612</v>
+      </c>
+      <c r="D437" t="s">
+        <v>3622</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A438" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B438" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="C438" s="16" t="s">
+        <v>3613</v>
+      </c>
+      <c r="D438" t="s">
+        <v>3618</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A439" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B439" s="3" t="s">
+        <v>3501</v>
+      </c>
+      <c r="C439" s="16" t="s">
+        <v>3624</v>
+      </c>
+      <c r="D439" t="s">
+        <v>3641</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A440" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B440" s="3" t="s">
+        <v>3501</v>
+      </c>
+      <c r="C440" s="16" t="s">
+        <v>3625</v>
+      </c>
+      <c r="D440" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A441" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B441" s="3" t="s">
+        <v>3501</v>
+      </c>
+      <c r="C441" s="16" t="s">
+        <v>3626</v>
+      </c>
+      <c r="D441" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A442" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B442" s="3" t="s">
+        <v>3501</v>
+      </c>
+      <c r="C442" s="16" t="s">
+        <v>3627</v>
+      </c>
+      <c r="D442" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A443" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B443" s="3" t="s">
+        <v>3501</v>
+      </c>
+      <c r="C443" s="16" t="s">
+        <v>3628</v>
+      </c>
+      <c r="D443" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A444" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B444" s="3" t="s">
+        <v>3501</v>
+      </c>
+      <c r="C444" s="16" t="s">
+        <v>3629</v>
+      </c>
+      <c r="D444" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A445" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B445" s="3" t="s">
+        <v>3507</v>
+      </c>
+      <c r="C445" s="16" t="s">
+        <v>3630</v>
+      </c>
+      <c r="D445" t="s">
+        <v>3642</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A446" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B446" s="3" t="s">
+        <v>3507</v>
+      </c>
+      <c r="C446" s="16" t="s">
+        <v>3631</v>
+      </c>
+      <c r="D446" t="s">
+        <v>3643</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A447" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B447" s="3" t="s">
+        <v>3507</v>
+      </c>
+      <c r="C447" s="16" t="s">
+        <v>3632</v>
+      </c>
+      <c r="D447" t="s">
+        <v>3644</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A448" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B448" s="3" t="s">
+        <v>3503</v>
+      </c>
+      <c r="C448" s="16" t="s">
+        <v>3633</v>
+      </c>
+      <c r="D448" t="s">
+        <v>3645</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A449" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B449" s="3" t="s">
+        <v>3510</v>
+      </c>
+      <c r="C449" s="16" t="s">
+        <v>3634</v>
+      </c>
+      <c r="D449" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A450" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B450" s="3" t="s">
+        <v>3510</v>
+      </c>
+      <c r="C450" s="16" t="s">
+        <v>3635</v>
+      </c>
+      <c r="D450" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A451" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B451" s="3" t="s">
+        <v>3510</v>
+      </c>
+      <c r="C451" s="16" t="s">
+        <v>3636</v>
+      </c>
+      <c r="D451" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A452" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B452" s="3" t="s">
+        <v>3510</v>
+      </c>
+      <c r="C452" s="16" t="s">
+        <v>3637</v>
+      </c>
+      <c r="D452" t="s">
+        <v>3646</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A453" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B453" s="3" t="s">
+        <v>3510</v>
+      </c>
+      <c r="C453" s="16" t="s">
+        <v>3638</v>
+      </c>
+      <c r="D453" t="s">
+        <v>3646</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A454" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B454" s="3" t="s">
+        <v>3510</v>
+      </c>
+      <c r="C454" s="16" t="s">
+        <v>3639</v>
+      </c>
+      <c r="D454" t="s">
+        <v>3646</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A455" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B455" s="3" t="s">
+        <v>3510</v>
+      </c>
+      <c r="C455" s="16" t="s">
+        <v>3640</v>
+      </c>
+      <c r="D455" t="s">
+        <v>3647</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A456" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B456" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="C456" s="16" t="s">
+        <v>3648</v>
+      </c>
+      <c r="D456" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A457" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B457" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="C457" s="16" t="s">
+        <v>3649</v>
+      </c>
+      <c r="D457" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A458" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B458" s="3" t="s">
+        <v>3545</v>
+      </c>
+      <c r="C458" s="16" t="s">
+        <v>3650</v>
+      </c>
+      <c r="D458" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A459" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B459" s="3" t="s">
+        <v>3545</v>
+      </c>
+      <c r="C459" s="16" t="s">
+        <v>3651</v>
+      </c>
+      <c r="D459" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A460" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B460" s="3" t="s">
+        <v>3545</v>
+      </c>
+      <c r="C460" s="16" t="s">
+        <v>3652</v>
+      </c>
+      <c r="D460" t="s">
+        <v>3672</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A461" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B461" s="3" t="s">
+        <v>3546</v>
+      </c>
+      <c r="C461" s="16" t="s">
+        <v>3653</v>
+      </c>
+      <c r="D461" t="s">
+        <v>3670</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A462" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B462" s="3" t="s">
+        <v>3548</v>
+      </c>
+      <c r="C462" s="16" t="s">
+        <v>3654</v>
+      </c>
+      <c r="D462" t="s">
+        <v>3553</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A463" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B463" s="3" t="s">
+        <v>3549</v>
+      </c>
+      <c r="C463" s="16" t="s">
+        <v>3655</v>
+      </c>
+      <c r="D463" t="s">
+        <v>3671</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A464" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B464" s="3" t="s">
+        <v>3554</v>
+      </c>
+      <c r="C464" s="16" t="s">
+        <v>3656</v>
+      </c>
+      <c r="D464" t="s">
+        <v>3673</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A465" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B465" s="3" t="s">
+        <v>3554</v>
+      </c>
+      <c r="C465" s="16" t="s">
+        <v>3657</v>
+      </c>
+      <c r="D465" t="s">
+        <v>3674</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A466" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B466" s="3" t="s">
+        <v>3554</v>
+      </c>
+      <c r="C466" s="16" t="s">
+        <v>3658</v>
+      </c>
+      <c r="D466" t="s">
+        <v>3675</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A467" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B467" s="3" t="s">
+        <v>3554</v>
+      </c>
+      <c r="C467" s="16" t="s">
+        <v>3659</v>
+      </c>
+      <c r="D467" t="s">
+        <v>3553</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A468" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B468" s="3" t="s">
+        <v>3554</v>
+      </c>
+      <c r="C468" s="16" t="s">
+        <v>3660</v>
+      </c>
+      <c r="D468" t="s">
+        <v>3553</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A469" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B469" s="3" t="s">
+        <v>3554</v>
+      </c>
+      <c r="C469" s="16" t="s">
+        <v>3661</v>
+      </c>
+      <c r="D469" t="s">
+        <v>3677</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A470" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B470" s="3" t="s">
+        <v>3554</v>
+      </c>
+      <c r="C470" s="16" t="s">
+        <v>3662</v>
+      </c>
+      <c r="D470" t="s">
+        <v>3676</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A471" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B471" s="3" t="s">
+        <v>3555</v>
+      </c>
+      <c r="C471" s="16" t="s">
+        <v>3663</v>
+      </c>
+      <c r="D471" t="s">
+        <v>3678</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A472" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B472" s="3" t="s">
+        <v>3555</v>
+      </c>
+      <c r="C472" s="16" t="s">
+        <v>3664</v>
+      </c>
+      <c r="D472" t="s">
+        <v>3680</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A473" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B473" s="3" t="s">
+        <v>3555</v>
+      </c>
+      <c r="C473" s="16" t="s">
+        <v>3665</v>
+      </c>
+      <c r="D473" t="s">
+        <v>3681</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A474" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B474" s="3" t="s">
+        <v>3555</v>
+      </c>
+      <c r="C474" s="16" t="s">
+        <v>3666</v>
+      </c>
+      <c r="D474" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A475" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B475" s="3" t="s">
+        <v>3555</v>
+      </c>
+      <c r="C475" s="16" t="s">
+        <v>3667</v>
+      </c>
+      <c r="D475" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A476" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B476" s="3" t="s">
+        <v>3564</v>
+      </c>
+      <c r="C476" s="16" t="s">
+        <v>3668</v>
+      </c>
+      <c r="D476" t="s">
+        <v>3679</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A477" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B477" s="3" t="s">
+        <v>3564</v>
+      </c>
+      <c r="C477" s="16" t="s">
+        <v>3669</v>
+      </c>
+      <c r="D477" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A478" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B478" s="3" t="s">
+        <v>3515</v>
+      </c>
+      <c r="C478" s="16" t="s">
+        <v>3682</v>
+      </c>
+      <c r="D478" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A479" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B479" s="3" t="s">
+        <v>3515</v>
+      </c>
+      <c r="C479" s="16" t="s">
+        <v>3683</v>
+      </c>
+      <c r="D479" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A480" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B480" s="3" t="s">
+        <v>3516</v>
+      </c>
+      <c r="C480" s="16" t="s">
+        <v>3684</v>
+      </c>
+      <c r="D480" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A481" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B481" s="3" t="s">
+        <v>3516</v>
+      </c>
+      <c r="C481" s="16" t="s">
+        <v>3685</v>
+      </c>
+      <c r="D481" t="s">
+        <v>3697</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A482" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B482" s="3" t="s">
+        <v>3516</v>
+      </c>
+      <c r="C482" s="16" t="s">
+        <v>3686</v>
+      </c>
+      <c r="D482" t="s">
+        <v>3697</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A483" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B483" s="3" t="s">
+        <v>3516</v>
+      </c>
+      <c r="C483" s="16" t="s">
+        <v>3687</v>
+      </c>
+      <c r="D483" t="s">
+        <v>3697</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A484" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B484" s="3" t="s">
+        <v>3516</v>
+      </c>
+      <c r="C484" s="16" t="s">
+        <v>3688</v>
+      </c>
+      <c r="D484" t="s">
+        <v>3697</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A485" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B485" s="3" t="s">
+        <v>3517</v>
+      </c>
+      <c r="C485" s="16" t="s">
+        <v>3689</v>
+      </c>
+      <c r="D485" t="s">
+        <v>3698</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A486" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B486" s="3" t="s">
+        <v>3517</v>
+      </c>
+      <c r="C486" s="16" t="s">
+        <v>3690</v>
+      </c>
+      <c r="D486" t="s">
+        <v>3699</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A487" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B487" s="3" t="s">
+        <v>3515</v>
+      </c>
+      <c r="C487" s="16" t="s">
+        <v>3691</v>
+      </c>
+      <c r="D487" t="s">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A488" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B488" s="3" t="s">
+        <v>3515</v>
+      </c>
+      <c r="C488" s="16" t="s">
+        <v>3692</v>
+      </c>
+      <c r="D488" t="s">
+        <v>3701</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A489" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B489" s="3" t="s">
+        <v>3515</v>
+      </c>
+      <c r="C489" s="16" t="s">
+        <v>3693</v>
+      </c>
+      <c r="D489" t="s">
+        <v>3702</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A490" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B490" s="3" t="s">
+        <v>3515</v>
+      </c>
+      <c r="C490" s="16" t="s">
+        <v>3694</v>
+      </c>
+      <c r="D490" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A491" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B491" s="3" t="s">
+        <v>3515</v>
+      </c>
+      <c r="C491" s="16" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D491" t="s">
+        <v>3703</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A492" s="10" t="s">
+        <v>3495</v>
+      </c>
+      <c r="B492" s="3" t="s">
+        <v>3515</v>
+      </c>
+      <c r="C492" s="16" t="s">
+        <v>3696</v>
+      </c>
+      <c r="D492" t="s">
+        <v>3701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Pulpit Rock Trail
</commit_message>
<xml_diff>
--- a/Data/Trail Mapping Info.xlsx
+++ b/Data/Trail Mapping Info.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10414" uniqueCount="3712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10490" uniqueCount="3741">
   <si>
     <t>trackID</t>
   </si>
@@ -11157,6 +11157,93 @@
   </si>
   <si>
     <t>South Jackman Lake Rd</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>PLPT01</t>
+  </si>
+  <si>
+    <t>Pulpit Rock Tr</t>
+  </si>
+  <si>
+    <t>PLPT02</t>
+  </si>
+  <si>
+    <t>PLPT03</t>
+  </si>
+  <si>
+    <t>PLPT04</t>
+  </si>
+  <si>
+    <t>PLPT05</t>
+  </si>
+  <si>
+    <t>PLPT06</t>
+  </si>
+  <si>
+    <t>PLPT07</t>
+  </si>
+  <si>
+    <t>PLPT08</t>
+  </si>
+  <si>
+    <t>PLPT02, PLPT05</t>
+  </si>
+  <si>
+    <t>PLPT01, PLPT05</t>
+  </si>
+  <si>
+    <t>PLPT03, PLPT06</t>
+  </si>
+  <si>
+    <t>PLPT02, PLPT06</t>
+  </si>
+  <si>
+    <t>PLPT04, PLPT07</t>
+  </si>
+  <si>
+    <t>PLPT03, PLPT07</t>
+  </si>
+  <si>
+    <t>PLPT01, PLPT02</t>
+  </si>
+  <si>
+    <t>PLPT02, PLPT03</t>
+  </si>
+  <si>
+    <t>PLPT07, PLPT08</t>
+  </si>
+  <si>
+    <t>PLPT06, PLPT08</t>
+  </si>
+  <si>
+    <t>PLTP07</t>
+  </si>
+  <si>
+    <t>Private Road</t>
+  </si>
+  <si>
+    <t>PLPT03, PLPT04</t>
+  </si>
+  <si>
+    <t>IMG_4337</t>
+  </si>
+  <si>
+    <t>IMG_4338</t>
+  </si>
+  <si>
+    <t>IMG_4340</t>
+  </si>
+  <si>
+    <t>IMG_4341</t>
+  </si>
+  <si>
+    <t>IMG_4343</t>
+  </si>
+  <si>
+    <t>IMG_4344</t>
   </si>
 </sst>
 </file>
@@ -11505,13 +11592,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X1032"/>
+  <dimension ref="A1:X1040"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1007" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1019" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="B1039" sqref="B1039"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -39266,6 +39353,196 @@
       </c>
       <c r="H1032" s="3" t="s">
         <v>3499</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1033" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1033" s="3" t="s">
+        <v>3713</v>
+      </c>
+      <c r="C1033" s="3" t="s">
+        <v>3714</v>
+      </c>
+      <c r="D1033" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1033" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1033" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="H1033" s="3" t="s">
+        <v>3717</v>
+      </c>
+      <c r="I1033" s="3" t="s">
+        <v>3722</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1034" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1034" s="3" t="s">
+        <v>3715</v>
+      </c>
+      <c r="C1034" s="3" t="s">
+        <v>3714</v>
+      </c>
+      <c r="D1034" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1034" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1034" s="3" t="s">
+        <v>3723</v>
+      </c>
+      <c r="I1034" s="3" t="s">
+        <v>3724</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1035" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1035" s="3" t="s">
+        <v>3716</v>
+      </c>
+      <c r="C1035" s="3" t="s">
+        <v>3714</v>
+      </c>
+      <c r="D1035" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1035" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1035" s="3" t="s">
+        <v>3725</v>
+      </c>
+      <c r="I1035" s="3" t="s">
+        <v>3726</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1036" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1036" s="3" t="s">
+        <v>3717</v>
+      </c>
+      <c r="C1036" s="3" t="s">
+        <v>3714</v>
+      </c>
+      <c r="D1036" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1036" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1036" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="H1036" s="3" t="s">
+        <v>3727</v>
+      </c>
+      <c r="I1036" s="3" t="s">
+        <v>3713</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1037" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1037" s="3" t="s">
+        <v>3718</v>
+      </c>
+      <c r="C1037" s="3" t="s">
+        <v>3714</v>
+      </c>
+      <c r="D1037" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1037" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1037" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="I1037" s="3" t="s">
+        <v>3728</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1038" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1038" s="3" t="s">
+        <v>3719</v>
+      </c>
+      <c r="C1038" s="3" t="s">
+        <v>3714</v>
+      </c>
+      <c r="D1038" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1038" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1038" s="3" t="s">
+        <v>3729</v>
+      </c>
+      <c r="I1038" s="3" t="s">
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1039" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1039" s="3" t="s">
+        <v>3720</v>
+      </c>
+      <c r="C1039" s="3" t="s">
+        <v>3714</v>
+      </c>
+      <c r="D1039" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1039" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1039" s="3" t="s">
+        <v>3731</v>
+      </c>
+      <c r="I1039" s="3" t="s">
+        <v>3734</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1040" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1040" s="3" t="s">
+        <v>3721</v>
+      </c>
+      <c r="C1040" s="3" t="s">
+        <v>3714</v>
+      </c>
+      <c r="D1040" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1040" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1040" s="3" t="s">
+        <v>3733</v>
+      </c>
+      <c r="H1040" s="3" t="s">
+        <v>3732</v>
       </c>
     </row>
   </sheetData>
@@ -65604,11 +65881,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z492"/>
+  <dimension ref="A1:Z498"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A479" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D488" sqref="D488"/>
+      <selection pane="bottomLeft" activeCell="B499" sqref="B499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -72545,6 +72822,72 @@
         <v>3695</v>
       </c>
     </row>
+    <row r="493" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A493" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B493" s="3" t="s">
+        <v>3715</v>
+      </c>
+      <c r="C493" s="16" t="s">
+        <v>3735</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A494" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B494" s="3" t="s">
+        <v>3715</v>
+      </c>
+      <c r="C494" s="16" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A495" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B495" s="3" t="s">
+        <v>3715</v>
+      </c>
+      <c r="C495" s="16" t="s">
+        <v>3737</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A496" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B496" s="3" t="s">
+        <v>3715</v>
+      </c>
+      <c r="C496" s="16" t="s">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A497" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B497" s="3" t="s">
+        <v>3715</v>
+      </c>
+      <c r="C497" s="16" t="s">
+        <v>3739</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A498" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B498" s="3" t="s">
+        <v>3717</v>
+      </c>
+      <c r="C498" s="16" t="s">
+        <v>3740</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Echo Valley Trail
</commit_message>
<xml_diff>
--- a/Data/Trail Mapping Info.xlsx
+++ b/Data/Trail Mapping Info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tracks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10490" uniqueCount="3741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10567" uniqueCount="3768">
   <si>
     <t>trackID</t>
   </si>
@@ -11228,9 +11228,6 @@
     <t>PLPT03, PLPT04</t>
   </si>
   <si>
-    <t>IMG_4337</t>
-  </si>
-  <si>
     <t>IMG_4338</t>
   </si>
   <si>
@@ -11244,6 +11241,90 @@
   </si>
   <si>
     <t>IMG_4344</t>
+  </si>
+  <si>
+    <t>Pulpit Rock from below</t>
+  </si>
+  <si>
+    <t>Pulpit Rock from above</t>
+  </si>
+  <si>
+    <t>Steps to view of Pulpit Rock</t>
+  </si>
+  <si>
+    <t>Panoramic view from above Pulpit Rock</t>
+  </si>
+  <si>
+    <t>Headed back down to the parking area</t>
+  </si>
+  <si>
+    <t>EVET01</t>
+  </si>
+  <si>
+    <t>EVET02</t>
+  </si>
+  <si>
+    <t>EVET03</t>
+  </si>
+  <si>
+    <t>EVET04</t>
+  </si>
+  <si>
+    <t>EVET05</t>
+  </si>
+  <si>
+    <t>Echo Valley Environmental Nature Trail</t>
+  </si>
+  <si>
+    <t>Parking area (near Echo Valley SP)</t>
+  </si>
+  <si>
+    <t>Echo Valley SP road</t>
+  </si>
+  <si>
+    <t>Unnamed trail</t>
+  </si>
+  <si>
+    <t>Glover's Creek trail</t>
+  </si>
+  <si>
+    <t>Picnic area</t>
+  </si>
+  <si>
+    <t>IMG_4399</t>
+  </si>
+  <si>
+    <t>IMG_4401</t>
+  </si>
+  <si>
+    <t>IMG_4402</t>
+  </si>
+  <si>
+    <t>IMG_4403</t>
+  </si>
+  <si>
+    <t>IMG_4404</t>
+  </si>
+  <si>
+    <t>Parking area at end of trail</t>
+  </si>
+  <si>
+    <t>Typical scenery in Winter 2023</t>
+  </si>
+  <si>
+    <t>Sign at parking area near Echo Valley SP</t>
+  </si>
+  <si>
+    <t>IMG_1850</t>
+  </si>
+  <si>
+    <t>IMG_1853</t>
+  </si>
+  <si>
+    <t>IMG_1861</t>
+  </si>
+  <si>
+    <t>Cash at Echo Valley State Park</t>
   </si>
 </sst>
 </file>
@@ -11592,13 +11673,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X1040"/>
+  <dimension ref="A1:X1045"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1019" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C1021" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1039" sqref="B1039"/>
+      <selection pane="bottomRight" activeCell="F1046" sqref="F1046"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -39543,6 +39624,145 @@
       </c>
       <c r="H1040" s="3" t="s">
         <v>3732</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1041" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1041" s="3" t="s">
+        <v>3745</v>
+      </c>
+      <c r="C1041" s="3" t="s">
+        <v>3750</v>
+      </c>
+      <c r="D1041" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1041" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1041" s="3" t="s">
+        <v>3751</v>
+      </c>
+      <c r="G1041" s="3" t="s">
+        <v>3752</v>
+      </c>
+      <c r="I1041" s="3" t="s">
+        <v>3746</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1042" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1042" s="3" t="s">
+        <v>3746</v>
+      </c>
+      <c r="C1042" s="3" t="s">
+        <v>3750</v>
+      </c>
+      <c r="D1042" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1042" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1042" s="3" t="s">
+        <v>3752</v>
+      </c>
+      <c r="G1042" s="3" t="s">
+        <v>3753</v>
+      </c>
+      <c r="H1042" s="3" t="s">
+        <v>3745</v>
+      </c>
+      <c r="I1042" s="3" t="s">
+        <v>3747</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1043" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1043" s="3" t="s">
+        <v>3747</v>
+      </c>
+      <c r="C1043" s="3" t="s">
+        <v>3750</v>
+      </c>
+      <c r="D1043" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1043" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1043" s="3" t="s">
+        <v>3753</v>
+      </c>
+      <c r="G1043" s="3" t="s">
+        <v>3754</v>
+      </c>
+      <c r="H1043" s="3" t="s">
+        <v>3746</v>
+      </c>
+      <c r="I1043" s="3" t="s">
+        <v>3748</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1044" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1044" s="3" t="s">
+        <v>3748</v>
+      </c>
+      <c r="C1044" s="3" t="s">
+        <v>3750</v>
+      </c>
+      <c r="D1044" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1044" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1044" s="3" t="s">
+        <v>3754</v>
+      </c>
+      <c r="G1044" s="3" t="s">
+        <v>3755</v>
+      </c>
+      <c r="H1044" s="3" t="s">
+        <v>3747</v>
+      </c>
+      <c r="I1044" s="3" t="s">
+        <v>3749</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1045" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1045" s="3" t="s">
+        <v>3749</v>
+      </c>
+      <c r="C1045" s="3" t="s">
+        <v>3750</v>
+      </c>
+      <c r="D1045" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1045" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1045" s="3" t="s">
+        <v>3755</v>
+      </c>
+      <c r="G1045" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="H1045" s="3" t="s">
+        <v>3748</v>
       </c>
     </row>
   </sheetData>
@@ -65881,11 +66101,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z498"/>
+  <dimension ref="A1:Z505"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A479" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B499" sqref="B499"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A481" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D505" sqref="D505"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -72832,6 +73052,9 @@
       <c r="C493" s="16" t="s">
         <v>3735</v>
       </c>
+      <c r="D493" t="s">
+        <v>3740</v>
+      </c>
     </row>
     <row r="494" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A494" s="10" t="s">
@@ -72843,6 +73066,9 @@
       <c r="C494" s="16" t="s">
         <v>3736</v>
       </c>
+      <c r="D494" t="s">
+        <v>3742</v>
+      </c>
     </row>
     <row r="495" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A495" s="10" t="s">
@@ -72854,6 +73080,9 @@
       <c r="C495" s="16" t="s">
         <v>3737</v>
       </c>
+      <c r="D495" t="s">
+        <v>3741</v>
+      </c>
     </row>
     <row r="496" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A496" s="10" t="s">
@@ -72865,27 +73094,134 @@
       <c r="C496" s="16" t="s">
         <v>3738</v>
       </c>
-    </row>
-    <row r="497" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D496" t="s">
+        <v>3743</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A497" s="10" t="s">
         <v>3712</v>
       </c>
       <c r="B497" s="3" t="s">
-        <v>3715</v>
+        <v>3717</v>
       </c>
       <c r="C497" s="16" t="s">
         <v>3739</v>
       </c>
-    </row>
-    <row r="498" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D497" t="s">
+        <v>3744</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A498" s="10" t="s">
         <v>3712</v>
       </c>
       <c r="B498" s="3" t="s">
-        <v>3717</v>
+        <v>3747</v>
       </c>
       <c r="C498" s="16" t="s">
-        <v>3740</v>
+        <v>3756</v>
+      </c>
+      <c r="D498" t="s">
+        <v>3762</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A499" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B499" s="3" t="s">
+        <v>3747</v>
+      </c>
+      <c r="C499" s="16" t="s">
+        <v>3757</v>
+      </c>
+      <c r="D499" t="s">
+        <v>3762</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A500" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B500" s="3" t="s">
+        <v>3749</v>
+      </c>
+      <c r="C500" s="16" t="s">
+        <v>3758</v>
+      </c>
+      <c r="D500" t="s">
+        <v>3761</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A501" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B501" s="3" t="s">
+        <v>3749</v>
+      </c>
+      <c r="C501" s="16" t="s">
+        <v>3759</v>
+      </c>
+      <c r="D501" t="s">
+        <v>3762</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A502" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B502" t="s">
+        <v>3745</v>
+      </c>
+      <c r="C502" s="16" t="s">
+        <v>3760</v>
+      </c>
+      <c r="D502" t="s">
+        <v>3763</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A503" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B503" s="3" t="s">
+        <v>3746</v>
+      </c>
+      <c r="C503" s="16" t="s">
+        <v>3764</v>
+      </c>
+      <c r="D503" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A504" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B504" s="3" t="s">
+        <v>3746</v>
+      </c>
+      <c r="C504" s="16" t="s">
+        <v>3765</v>
+      </c>
+      <c r="D504" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A505" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B505" s="3" t="s">
+        <v>3745</v>
+      </c>
+      <c r="C505" s="16" t="s">
+        <v>3766</v>
+      </c>
+      <c r="D505" t="s">
+        <v>3767</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more IA info
</commit_message>
<xml_diff>
--- a/Data/Trail Mapping Info.xlsx
+++ b/Data/Trail Mapping Info.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10567" uniqueCount="3768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10755" uniqueCount="3832">
   <si>
     <t>trackID</t>
   </si>
@@ -11325,6 +11325,198 @@
   </si>
   <si>
     <t>Cash at Echo Valley State Park</t>
+  </si>
+  <si>
+    <t>BHRN01</t>
+  </si>
+  <si>
+    <t>Bighorn Rd</t>
+  </si>
+  <si>
+    <t>W51</t>
+  </si>
+  <si>
+    <t>US 56</t>
+  </si>
+  <si>
+    <t>Need from W51 to Pops'</t>
+  </si>
+  <si>
+    <t>Backbone SP - North Gate Rd</t>
+  </si>
+  <si>
+    <t>North Gate</t>
+  </si>
+  <si>
+    <t>Richmond Springs trail</t>
+  </si>
+  <si>
+    <t>Barred Owl trail [North]</t>
+  </si>
+  <si>
+    <t>Cave trail</t>
+  </si>
+  <si>
+    <t>Barred Owl trail [South]</t>
+  </si>
+  <si>
+    <t>South Flats trail</t>
+  </si>
+  <si>
+    <t>East Gate Rd</t>
+  </si>
+  <si>
+    <t>BBBOT01</t>
+  </si>
+  <si>
+    <t>BBBOT02</t>
+  </si>
+  <si>
+    <t>Backbone SP - Barred Owl Tr</t>
+  </si>
+  <si>
+    <t>North Gate Rd</t>
+  </si>
+  <si>
+    <t>overlook</t>
+  </si>
+  <si>
+    <t>BBSFT01</t>
+  </si>
+  <si>
+    <t>BBSFT02</t>
+  </si>
+  <si>
+    <t>Backbone SP - South Flats Tr</t>
+  </si>
+  <si>
+    <t>Six Pines Tr</t>
+  </si>
+  <si>
+    <t>BBNGR01</t>
+  </si>
+  <si>
+    <t>BBNGR02</t>
+  </si>
+  <si>
+    <t>BBNGR03</t>
+  </si>
+  <si>
+    <t>BBNGR04</t>
+  </si>
+  <si>
+    <t>BBNGR05</t>
+  </si>
+  <si>
+    <t>BBNGR06</t>
+  </si>
+  <si>
+    <t>BBNGR02, BBGR03</t>
+  </si>
+  <si>
+    <t>BBNGR04, BBNGR05</t>
+  </si>
+  <si>
+    <t>BBNGR05, BBNGR05</t>
+  </si>
+  <si>
+    <t>PNYH01</t>
+  </si>
+  <si>
+    <t>Pony Hollow Tr</t>
+  </si>
+  <si>
+    <t>South High St (Elkader)</t>
+  </si>
+  <si>
+    <t>Grape Rd</t>
+  </si>
+  <si>
+    <t>Can be continued from Grape Rd</t>
+  </si>
+  <si>
+    <t>GRWD40</t>
+  </si>
+  <si>
+    <t>GRWD41</t>
+  </si>
+  <si>
+    <t>GRWD42</t>
+  </si>
+  <si>
+    <t>GRWD43</t>
+  </si>
+  <si>
+    <t>GRWD44</t>
+  </si>
+  <si>
+    <t>Grant Wood Tr</t>
+  </si>
+  <si>
+    <t>Oxley Rd</t>
+  </si>
+  <si>
+    <t>Hindman Rd</t>
+  </si>
+  <si>
+    <t>Waldo's Rock Park</t>
+  </si>
+  <si>
+    <t>62nd St parking</t>
+  </si>
+  <si>
+    <t>Hwy 13/151 Tunnel</t>
+  </si>
+  <si>
+    <t>44th St</t>
+  </si>
+  <si>
+    <t>IMG_4370</t>
+  </si>
+  <si>
+    <t>Waldo's Rock</t>
+  </si>
+  <si>
+    <t>IMG_1870</t>
+  </si>
+  <si>
+    <t>IMG_1872</t>
+  </si>
+  <si>
+    <t>IMG_4376</t>
+  </si>
+  <si>
+    <t>IMG_4377</t>
+  </si>
+  <si>
+    <t>IMG_4379</t>
+  </si>
+  <si>
+    <t>IMG_4380</t>
+  </si>
+  <si>
+    <t>IMG_4386</t>
+  </si>
+  <si>
+    <t>Balance Rock</t>
+  </si>
+  <si>
+    <t>Cash near Richmond Springs</t>
+  </si>
+  <si>
+    <t>BBXXXX</t>
+  </si>
+  <si>
+    <t>Cash at Backbone Cave</t>
+  </si>
+  <si>
+    <t>IMG_1886</t>
+  </si>
+  <si>
+    <t>IMG_1888</t>
+  </si>
+  <si>
+    <t>IMG_1894</t>
   </si>
 </sst>
 </file>
@@ -11673,13 +11865,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X1045"/>
+  <dimension ref="A1:X1062"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C1021" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1028" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1046" sqref="F1046"/>
+      <selection pane="bottomRight" activeCell="B1057" sqref="B1057"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -39626,7 +39818,7 @@
         <v>3732</v>
       </c>
     </row>
-    <row r="1041" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1041" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1041" s="3" t="s">
         <v>3712</v>
       </c>
@@ -39652,7 +39844,7 @@
         <v>3746</v>
       </c>
     </row>
-    <row r="1042" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1042" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1042" s="3" t="s">
         <v>3712</v>
       </c>
@@ -39681,7 +39873,7 @@
         <v>3747</v>
       </c>
     </row>
-    <row r="1043" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1043" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1043" s="3" t="s">
         <v>3712</v>
       </c>
@@ -39710,7 +39902,7 @@
         <v>3748</v>
       </c>
     </row>
-    <row r="1044" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1044" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1044" s="3" t="s">
         <v>3712</v>
       </c>
@@ -39739,7 +39931,7 @@
         <v>3749</v>
       </c>
     </row>
-    <row r="1045" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1045" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1045" s="3" t="s">
         <v>3712</v>
       </c>
@@ -39763,6 +39955,472 @@
       </c>
       <c r="H1045" s="3" t="s">
         <v>3748</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1046" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1046" s="3" t="s">
+        <v>3768</v>
+      </c>
+      <c r="C1046" s="3" t="s">
+        <v>3769</v>
+      </c>
+      <c r="D1046" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1046" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1046" s="3" t="s">
+        <v>3770</v>
+      </c>
+      <c r="G1046" s="3" t="s">
+        <v>3771</v>
+      </c>
+      <c r="J1046" s="3" t="s">
+        <v>3772</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1047" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1047" s="3" t="s">
+        <v>3790</v>
+      </c>
+      <c r="C1047" s="3" t="s">
+        <v>3773</v>
+      </c>
+      <c r="D1047" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1047" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1047" s="3" t="s">
+        <v>3774</v>
+      </c>
+      <c r="G1047" s="3" t="s">
+        <v>3775</v>
+      </c>
+      <c r="I1047" s="3" t="s">
+        <v>3791</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1048" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1048" s="3" t="s">
+        <v>3791</v>
+      </c>
+      <c r="C1048" s="3" t="s">
+        <v>3773</v>
+      </c>
+      <c r="D1048" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1048" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1048" s="3" t="s">
+        <v>3775</v>
+      </c>
+      <c r="G1048" s="3" t="s">
+        <v>3776</v>
+      </c>
+      <c r="H1048" s="3" t="s">
+        <v>3790</v>
+      </c>
+      <c r="I1048" s="3" t="s">
+        <v>3792</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1049" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1049" s="3" t="s">
+        <v>3792</v>
+      </c>
+      <c r="C1049" s="3" t="s">
+        <v>3773</v>
+      </c>
+      <c r="D1049" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1049" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1049" s="3" t="s">
+        <v>3776</v>
+      </c>
+      <c r="G1049" s="3" t="s">
+        <v>3777</v>
+      </c>
+      <c r="H1049" s="3" t="s">
+        <v>3791</v>
+      </c>
+      <c r="I1049" s="3" t="s">
+        <v>3793</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1050" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1050" s="3" t="s">
+        <v>3793</v>
+      </c>
+      <c r="C1050" s="3" t="s">
+        <v>3773</v>
+      </c>
+      <c r="D1050" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1050" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1050" s="3" t="s">
+        <v>3777</v>
+      </c>
+      <c r="G1050" s="3" t="s">
+        <v>3778</v>
+      </c>
+      <c r="H1050" s="3" t="s">
+        <v>3792</v>
+      </c>
+      <c r="I1050" s="3" t="s">
+        <v>3794</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1051" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1051" s="3" t="s">
+        <v>3794</v>
+      </c>
+      <c r="C1051" s="3" t="s">
+        <v>3773</v>
+      </c>
+      <c r="D1051" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1051" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1051" s="3" t="s">
+        <v>3778</v>
+      </c>
+      <c r="G1051" s="3" t="s">
+        <v>3779</v>
+      </c>
+      <c r="H1051" s="3" t="s">
+        <v>3793</v>
+      </c>
+      <c r="I1051" s="3" t="s">
+        <v>3795</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1052" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1052" s="3" t="s">
+        <v>3795</v>
+      </c>
+      <c r="C1052" s="3" t="s">
+        <v>3773</v>
+      </c>
+      <c r="D1052" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1052" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1052" s="3" t="s">
+        <v>3779</v>
+      </c>
+      <c r="G1052" s="3" t="s">
+        <v>3780</v>
+      </c>
+      <c r="H1052" s="3" t="s">
+        <v>3794</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1053" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1053" s="3" t="s">
+        <v>3781</v>
+      </c>
+      <c r="C1053" s="3" t="s">
+        <v>3783</v>
+      </c>
+      <c r="D1053" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1053" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1053" s="3" t="s">
+        <v>3784</v>
+      </c>
+      <c r="G1053" s="3" t="s">
+        <v>3785</v>
+      </c>
+      <c r="H1053" s="3" t="s">
+        <v>3796</v>
+      </c>
+      <c r="I1053" s="3" t="s">
+        <v>3782</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1054" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1054" s="3" t="s">
+        <v>3782</v>
+      </c>
+      <c r="C1054" s="3" t="s">
+        <v>3783</v>
+      </c>
+      <c r="D1054" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1054" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1054" s="3" t="s">
+        <v>3785</v>
+      </c>
+      <c r="G1054" s="3" t="s">
+        <v>3784</v>
+      </c>
+      <c r="H1054" s="3" t="s">
+        <v>3781</v>
+      </c>
+      <c r="I1054" s="3" t="s">
+        <v>3797</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1055" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1055" s="3" t="s">
+        <v>3786</v>
+      </c>
+      <c r="C1055" s="3" t="s">
+        <v>3788</v>
+      </c>
+      <c r="D1055" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1055" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1055" s="3" t="s">
+        <v>3784</v>
+      </c>
+      <c r="G1055" s="3" t="s">
+        <v>3789</v>
+      </c>
+      <c r="H1055" s="3" t="s">
+        <v>3798</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1056" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1056" s="3" t="s">
+        <v>3787</v>
+      </c>
+      <c r="C1056" s="3" t="s">
+        <v>3788</v>
+      </c>
+      <c r="D1056" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1056" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1056" s="3" t="s">
+        <v>3789</v>
+      </c>
+      <c r="G1056" s="3" t="s">
+        <v>3780</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1057" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1057" s="3" t="s">
+        <v>3799</v>
+      </c>
+      <c r="C1057" s="3" t="s">
+        <v>3800</v>
+      </c>
+      <c r="D1057" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1057" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1057" s="3" t="s">
+        <v>3801</v>
+      </c>
+      <c r="G1057" s="3" t="s">
+        <v>3802</v>
+      </c>
+      <c r="J1057" s="3" t="s">
+        <v>3803</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1058" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1058" s="3" t="s">
+        <v>3804</v>
+      </c>
+      <c r="C1058" s="3" t="s">
+        <v>3809</v>
+      </c>
+      <c r="D1058" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1058" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1058" s="3" t="s">
+        <v>3815</v>
+      </c>
+      <c r="G1058" s="3" t="s">
+        <v>3814</v>
+      </c>
+      <c r="I1058" s="3" t="s">
+        <v>3805</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1059" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1059" s="3" t="s">
+        <v>3805</v>
+      </c>
+      <c r="C1059" s="3" t="s">
+        <v>3809</v>
+      </c>
+      <c r="D1059" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1059" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1059" s="3" t="s">
+        <v>3814</v>
+      </c>
+      <c r="G1059" s="3" t="s">
+        <v>3813</v>
+      </c>
+      <c r="H1059" s="3" t="s">
+        <v>3804</v>
+      </c>
+      <c r="I1059" s="3" t="s">
+        <v>3806</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1060" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1060" s="3" t="s">
+        <v>3806</v>
+      </c>
+      <c r="C1060" s="3" t="s">
+        <v>3809</v>
+      </c>
+      <c r="D1060" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1060" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1060" s="3" t="s">
+        <v>3813</v>
+      </c>
+      <c r="G1060" s="3" t="s">
+        <v>3812</v>
+      </c>
+      <c r="H1060" s="3" t="s">
+        <v>3805</v>
+      </c>
+      <c r="I1060" s="3" t="s">
+        <v>3807</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1061" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1061" s="3" t="s">
+        <v>3807</v>
+      </c>
+      <c r="C1061" s="3" t="s">
+        <v>3809</v>
+      </c>
+      <c r="D1061" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1061" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1061" s="3" t="s">
+        <v>3812</v>
+      </c>
+      <c r="G1061" s="3" t="s">
+        <v>3811</v>
+      </c>
+      <c r="H1061" s="3" t="s">
+        <v>3806</v>
+      </c>
+      <c r="I1061" s="3" t="s">
+        <v>3808</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1062" s="3" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B1062" s="3" t="s">
+        <v>3808</v>
+      </c>
+      <c r="C1062" s="3" t="s">
+        <v>3809</v>
+      </c>
+      <c r="D1062" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1062" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1062" s="3" t="s">
+        <v>3811</v>
+      </c>
+      <c r="G1062" s="3" t="s">
+        <v>3810</v>
+      </c>
+      <c r="H1062" s="3" t="s">
+        <v>3807</v>
       </c>
     </row>
   </sheetData>
@@ -66101,11 +66759,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z505"/>
+  <dimension ref="A1:Z516"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A481" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D505" sqref="D505"/>
+      <pane ySplit="1" topLeftCell="A492" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C516" sqref="C516"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -73224,6 +73882,160 @@
         <v>3767</v>
       </c>
     </row>
+    <row r="506" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A506" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B506" s="3" t="s">
+        <v>3806</v>
+      </c>
+      <c r="C506" s="16" t="s">
+        <v>3816</v>
+      </c>
+      <c r="D506" t="s">
+        <v>3817</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A507" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B507" s="3" t="s">
+        <v>3799</v>
+      </c>
+      <c r="C507" s="16" t="s">
+        <v>3818</v>
+      </c>
+      <c r="D507" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="508" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A508" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B508" s="3" t="s">
+        <v>3799</v>
+      </c>
+      <c r="C508" s="16" t="s">
+        <v>3819</v>
+      </c>
+      <c r="D508" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="509" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A509" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B509" s="3" t="s">
+        <v>3790</v>
+      </c>
+      <c r="C509" s="16" t="s">
+        <v>3820</v>
+      </c>
+      <c r="D509" t="s">
+        <v>3762</v>
+      </c>
+    </row>
+    <row r="510" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A510" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B510" s="3" t="s">
+        <v>3792</v>
+      </c>
+      <c r="C510" s="16" t="s">
+        <v>3821</v>
+      </c>
+      <c r="D510" t="s">
+        <v>3825</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A511" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B511" s="3" t="s">
+        <v>3794</v>
+      </c>
+      <c r="C511" s="16" t="s">
+        <v>3822</v>
+      </c>
+      <c r="D511" t="s">
+        <v>3762</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A512" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B512" s="3" t="s">
+        <v>3794</v>
+      </c>
+      <c r="C512" s="16" t="s">
+        <v>3823</v>
+      </c>
+      <c r="D512" t="s">
+        <v>3762</v>
+      </c>
+    </row>
+    <row r="513" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A513" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B513" s="3" t="s">
+        <v>3791</v>
+      </c>
+      <c r="C513" s="16" t="s">
+        <v>3824</v>
+      </c>
+      <c r="D513" t="s">
+        <v>3826</v>
+      </c>
+    </row>
+    <row r="514" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A514" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B514" s="3" t="s">
+        <v>3786</v>
+      </c>
+      <c r="C514" s="16" t="s">
+        <v>3829</v>
+      </c>
+      <c r="D514" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="515" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A515" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B515" s="3" t="s">
+        <v>3787</v>
+      </c>
+      <c r="C515" s="16" t="s">
+        <v>3830</v>
+      </c>
+      <c r="D515" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="516" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A516" s="10" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B516" s="3" t="s">
+        <v>3827</v>
+      </c>
+      <c r="C516" s="16" t="s">
+        <v>3831</v>
+      </c>
+      <c r="D516" t="s">
+        <v>3828</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Robbers Roost hike
</commit_message>
<xml_diff>
--- a/Data/Trail Mapping Info.xlsx
+++ b/Data/Trail Mapping Info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Tracks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11971" uniqueCount="4165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12132" uniqueCount="4231">
   <si>
     <t>trackID</t>
   </si>
@@ -12516,6 +12516,204 @@
   </si>
   <si>
     <t>IMG_5081</t>
+  </si>
+  <si>
+    <t>RBRR01</t>
+  </si>
+  <si>
+    <t>RBRR02</t>
+  </si>
+  <si>
+    <t>RBRR03</t>
+  </si>
+  <si>
+    <t>RBRR04</t>
+  </si>
+  <si>
+    <t>RBRR05</t>
+  </si>
+  <si>
+    <t>RBRR06</t>
+  </si>
+  <si>
+    <t>RBRR07</t>
+  </si>
+  <si>
+    <t>RBRR08</t>
+  </si>
+  <si>
+    <t>RBRR09</t>
+  </si>
+  <si>
+    <t>RBRR10</t>
+  </si>
+  <si>
+    <t>RBRR11</t>
+  </si>
+  <si>
+    <t>RBRR12</t>
+  </si>
+  <si>
+    <t>RBRR13</t>
+  </si>
+  <si>
+    <t>Wave Cave Tr</t>
+  </si>
+  <si>
+    <t>Robber's Roost Hike (Lost Goldmine Tr East)</t>
+  </si>
+  <si>
+    <t>Robber's Roost Hike (Carney Springs Tr)</t>
+  </si>
+  <si>
+    <t>False summit</t>
+  </si>
+  <si>
+    <t>Robber's Roost Hike (Carney Springs / Superstition Ridgeline Tr)</t>
+  </si>
+  <si>
+    <t>leave Carney Springs / Superstition Ridgeline Tr</t>
+  </si>
+  <si>
+    <t>start Robber's Roost Tr</t>
+  </si>
+  <si>
+    <t>Robber's Roost Hike (Robber's Roost Tr)</t>
+  </si>
+  <si>
+    <t>spur to Robber's Roost</t>
+  </si>
+  <si>
+    <t>arrive Robber's Roost</t>
+  </si>
+  <si>
+    <t>arrive Fremont Saddle / leave Robber's Roost Tr</t>
+  </si>
+  <si>
+    <t>Robber's Roost Hike (Cave Tr)</t>
+  </si>
+  <si>
+    <t>Geronimo Cave</t>
+  </si>
+  <si>
+    <t>arrive Peralta TH / leave Dutchman's Tr</t>
+  </si>
+  <si>
+    <t>leave Bluff Spring Tr</t>
+  </si>
+  <si>
+    <t>Robber's Roost Hike (Bluff Spring Tr (235))</t>
+  </si>
+  <si>
+    <t>Robber's Roost Hike (Dutchman's Tr (104))</t>
+  </si>
+  <si>
+    <t>start Peralta Rd</t>
+  </si>
+  <si>
+    <t>arrive Lost Goldmine East TH</t>
+  </si>
+  <si>
+    <t>Robber's Roost Hike (Peralta Rd)</t>
+  </si>
+  <si>
+    <t>IMG_5122</t>
+  </si>
+  <si>
+    <t>Looking up Carney Sprngs Tr</t>
+  </si>
+  <si>
+    <t>IMG_5127</t>
+  </si>
+  <si>
+    <t>On Carney Springs Tr</t>
+  </si>
+  <si>
+    <t>IMG_5130</t>
+  </si>
+  <si>
+    <t>IMG_5132</t>
+  </si>
+  <si>
+    <t>View down from false summit</t>
+  </si>
+  <si>
+    <t>IMG_5134</t>
+  </si>
+  <si>
+    <t>IMG_5140</t>
+  </si>
+  <si>
+    <t>View down from summit</t>
+  </si>
+  <si>
+    <t>IMG_5142</t>
+  </si>
+  <si>
+    <t>Looking east across ridgeline</t>
+  </si>
+  <si>
+    <t>Nearing Robber's Roost from the west</t>
+  </si>
+  <si>
+    <t>IMG_5147</t>
+  </si>
+  <si>
+    <t>IMG_5149</t>
+  </si>
+  <si>
+    <t>First passage to entering Robber's Roost</t>
+  </si>
+  <si>
+    <t>IMG_5151</t>
+  </si>
+  <si>
+    <t>Entrance to Robber's Roost</t>
+  </si>
+  <si>
+    <t>Waterfall in Robber's Roost</t>
+  </si>
+  <si>
+    <t>IMG_5153</t>
+  </si>
+  <si>
+    <t>Looking southeast out of Robber's Roost</t>
+  </si>
+  <si>
+    <t>IMG_5157</t>
+  </si>
+  <si>
+    <t>IMG_5158</t>
+  </si>
+  <si>
+    <t>Weaver's Needle</t>
+  </si>
+  <si>
+    <t>IMG_5161</t>
+  </si>
+  <si>
+    <t>Looking down on the Peralta Tr</t>
+  </si>
+  <si>
+    <t>Looking east across Peralta Canyon</t>
+  </si>
+  <si>
+    <t>IMG_5163</t>
+  </si>
+  <si>
+    <t>IMG_5165</t>
+  </si>
+  <si>
+    <t>Looking south down Peralta Canyon</t>
+  </si>
+  <si>
+    <t>Looking north up Peralta Canyon</t>
+  </si>
+  <si>
+    <t>IMG_5166</t>
+  </si>
+  <si>
+    <t>IMG_5174</t>
   </si>
 </sst>
 </file>
@@ -12864,13 +13062,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X1186"/>
+  <dimension ref="A1:X1200"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1156" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B1170" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1172" sqref="A1172:XFD1172"/>
+      <selection pane="bottomRight" activeCell="D1187" sqref="D1187:D1199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -43960,6 +44158,9 @@
       <c r="G1149" s="3" t="s">
         <v>3509</v>
       </c>
+      <c r="H1149" s="3" t="s">
+        <v>3531</v>
+      </c>
       <c r="I1149" s="3" t="s">
         <v>3533</v>
       </c>
@@ -44355,6 +44556,9 @@
       <c r="G1163" s="3" t="s">
         <v>3529</v>
       </c>
+      <c r="H1163" s="3" t="s">
+        <v>4078</v>
+      </c>
       <c r="I1163" s="3" t="s">
         <v>4069</v>
       </c>
@@ -44645,6 +44849,9 @@
       <c r="H1173" s="3" t="s">
         <v>4077</v>
       </c>
+      <c r="I1173" s="3" t="s">
+        <v>4068</v>
+      </c>
     </row>
     <row r="1174" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1174" s="3" t="s">
@@ -45003,6 +45210,386 @@
       <c r="H1186" s="3" t="s">
         <v>3489</v>
       </c>
+    </row>
+    <row r="1187" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1187" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1187" s="3" t="s">
+        <v>4165</v>
+      </c>
+      <c r="C1187" s="3" t="s">
+        <v>4179</v>
+      </c>
+      <c r="D1187">
+        <v>2023</v>
+      </c>
+      <c r="E1187" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1187" s="3" t="s">
+        <v>4079</v>
+      </c>
+      <c r="G1187" s="3" t="s">
+        <v>3491</v>
+      </c>
+      <c r="H1187" s="3" t="s">
+        <v>4177</v>
+      </c>
+      <c r="I1187" s="3" t="s">
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1188" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1188" s="3" t="s">
+        <v>4166</v>
+      </c>
+      <c r="C1188" s="3" t="s">
+        <v>4179</v>
+      </c>
+      <c r="D1188">
+        <v>2023</v>
+      </c>
+      <c r="E1188" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1188" s="3" t="s">
+        <v>3491</v>
+      </c>
+      <c r="G1188" s="3" t="s">
+        <v>4100</v>
+      </c>
+      <c r="H1188" s="3" t="s">
+        <v>4165</v>
+      </c>
+      <c r="I1188" s="3" t="s">
+        <v>4167</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1189" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1189" s="3" t="s">
+        <v>4167</v>
+      </c>
+      <c r="C1189" s="3" t="s">
+        <v>4180</v>
+      </c>
+      <c r="D1189">
+        <v>2023</v>
+      </c>
+      <c r="E1189" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1189" s="3" t="s">
+        <v>4101</v>
+      </c>
+      <c r="G1189" s="3" t="s">
+        <v>4178</v>
+      </c>
+      <c r="H1189" s="3" t="s">
+        <v>4166</v>
+      </c>
+      <c r="I1189" s="3" t="s">
+        <v>4168</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1190" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1190" s="3" t="s">
+        <v>4168</v>
+      </c>
+      <c r="C1190" s="3" t="s">
+        <v>4180</v>
+      </c>
+      <c r="D1190">
+        <v>2023</v>
+      </c>
+      <c r="E1190" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1190" s="3" t="s">
+        <v>4178</v>
+      </c>
+      <c r="G1190" s="3" t="s">
+        <v>4181</v>
+      </c>
+      <c r="H1190" s="3" t="s">
+        <v>4167</v>
+      </c>
+      <c r="I1190" s="3" t="s">
+        <v>4169</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1191" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1191" s="3" t="s">
+        <v>4169</v>
+      </c>
+      <c r="C1191" s="3" t="s">
+        <v>4182</v>
+      </c>
+      <c r="D1191">
+        <v>2023</v>
+      </c>
+      <c r="E1191" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1191" s="3" t="s">
+        <v>4181</v>
+      </c>
+      <c r="G1191" s="3" t="s">
+        <v>4183</v>
+      </c>
+      <c r="H1191" s="3" t="s">
+        <v>4168</v>
+      </c>
+      <c r="I1191" s="3" t="s">
+        <v>4170</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1192" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1192" s="3" t="s">
+        <v>4170</v>
+      </c>
+      <c r="C1192" s="3" t="s">
+        <v>4185</v>
+      </c>
+      <c r="D1192">
+        <v>2023</v>
+      </c>
+      <c r="E1192" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1192" s="3" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G1192" s="3" t="s">
+        <v>4186</v>
+      </c>
+      <c r="H1192" s="3" t="s">
+        <v>4169</v>
+      </c>
+      <c r="I1192" s="3" t="s">
+        <v>4171</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1193" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1193" s="3" t="s">
+        <v>4171</v>
+      </c>
+      <c r="C1193" s="3" t="s">
+        <v>4185</v>
+      </c>
+      <c r="D1193">
+        <v>2023</v>
+      </c>
+      <c r="E1193" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1193" s="3" t="s">
+        <v>4186</v>
+      </c>
+      <c r="G1193" s="3" t="s">
+        <v>4187</v>
+      </c>
+      <c r="H1193" s="3" t="s">
+        <v>4170</v>
+      </c>
+      <c r="I1193" s="3" t="s">
+        <v>4172</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1194" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1194" s="3" t="s">
+        <v>4172</v>
+      </c>
+      <c r="C1194" s="3" t="s">
+        <v>4185</v>
+      </c>
+      <c r="D1194">
+        <v>2023</v>
+      </c>
+      <c r="E1194" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1194" s="3" t="s">
+        <v>4186</v>
+      </c>
+      <c r="G1194" s="3" t="s">
+        <v>4188</v>
+      </c>
+      <c r="H1194" s="3" t="s">
+        <v>4171</v>
+      </c>
+      <c r="I1194" s="3" t="s">
+        <v>4173</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1195" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1195" s="3" t="s">
+        <v>4173</v>
+      </c>
+      <c r="C1195" s="3" t="s">
+        <v>4189</v>
+      </c>
+      <c r="D1195">
+        <v>2023</v>
+      </c>
+      <c r="E1195" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1195" s="3" t="s">
+        <v>4114</v>
+      </c>
+      <c r="G1195" s="3" t="s">
+        <v>4190</v>
+      </c>
+      <c r="H1195" s="3" t="s">
+        <v>4172</v>
+      </c>
+      <c r="I1195" s="3" t="s">
+        <v>4174</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1196" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1196" s="3" t="s">
+        <v>4174</v>
+      </c>
+      <c r="C1196" s="3" t="s">
+        <v>4189</v>
+      </c>
+      <c r="D1196">
+        <v>2023</v>
+      </c>
+      <c r="E1196" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1196" s="3" t="s">
+        <v>4190</v>
+      </c>
+      <c r="G1196" s="3" t="s">
+        <v>4115</v>
+      </c>
+      <c r="H1196" s="3" t="s">
+        <v>4173</v>
+      </c>
+      <c r="I1196" s="3" t="s">
+        <v>4175</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1197" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1197" s="3" t="s">
+        <v>4175</v>
+      </c>
+      <c r="C1197" s="3" t="s">
+        <v>4193</v>
+      </c>
+      <c r="D1197">
+        <v>2023</v>
+      </c>
+      <c r="E1197" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1197" s="3" t="s">
+        <v>4118</v>
+      </c>
+      <c r="G1197" s="3" t="s">
+        <v>4192</v>
+      </c>
+      <c r="H1197" s="3" t="s">
+        <v>4174</v>
+      </c>
+      <c r="I1197" s="3" t="s">
+        <v>4176</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1198" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1198" s="3" t="s">
+        <v>4176</v>
+      </c>
+      <c r="C1198" s="3" t="s">
+        <v>4194</v>
+      </c>
+      <c r="D1198">
+        <v>2023</v>
+      </c>
+      <c r="E1198" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1198" s="3" t="s">
+        <v>4122</v>
+      </c>
+      <c r="G1198" s="3" t="s">
+        <v>4191</v>
+      </c>
+      <c r="H1198" s="3" t="s">
+        <v>4175</v>
+      </c>
+      <c r="I1198" s="3" t="s">
+        <v>4177</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1199" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1199" s="3" t="s">
+        <v>4177</v>
+      </c>
+      <c r="C1199" s="3" t="s">
+        <v>4197</v>
+      </c>
+      <c r="D1199">
+        <v>2023</v>
+      </c>
+      <c r="E1199" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1199" s="3" t="s">
+        <v>4195</v>
+      </c>
+      <c r="G1199" s="3" t="s">
+        <v>4196</v>
+      </c>
+      <c r="H1199" s="3" t="s">
+        <v>4176</v>
+      </c>
+      <c r="I1199" s="3" t="s">
+        <v>4165</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1200" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A2:X1186">
@@ -71340,11 +71927,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z551"/>
+  <dimension ref="A1:Z569"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A528" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C543" sqref="C543"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A547" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C570" sqref="C570"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -79056,6 +79643,204 @@
         <v>4162</v>
       </c>
     </row>
+    <row r="552" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B552" s="16" t="s">
+        <v>4168</v>
+      </c>
+      <c r="C552" s="16" t="s">
+        <v>4198</v>
+      </c>
+      <c r="D552" t="s">
+        <v>4199</v>
+      </c>
+    </row>
+    <row r="553" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B553" s="16" t="s">
+        <v>4168</v>
+      </c>
+      <c r="C553" s="16" t="s">
+        <v>4200</v>
+      </c>
+      <c r="D553" t="s">
+        <v>4201</v>
+      </c>
+    </row>
+    <row r="554" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B554" s="16" t="s">
+        <v>4168</v>
+      </c>
+      <c r="C554" s="16" t="s">
+        <v>4202</v>
+      </c>
+      <c r="D554" t="s">
+        <v>4199</v>
+      </c>
+    </row>
+    <row r="555" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B555" s="16" t="s">
+        <v>4168</v>
+      </c>
+      <c r="C555" s="16" t="s">
+        <v>4203</v>
+      </c>
+      <c r="D555" t="s">
+        <v>4199</v>
+      </c>
+    </row>
+    <row r="556" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B556" s="16" t="s">
+        <v>4169</v>
+      </c>
+      <c r="C556" s="16" t="s">
+        <v>4205</v>
+      </c>
+      <c r="D556" t="s">
+        <v>4204</v>
+      </c>
+    </row>
+    <row r="557" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B557" s="16" t="s">
+        <v>4170</v>
+      </c>
+      <c r="C557" s="16" t="s">
+        <v>4206</v>
+      </c>
+      <c r="D557" t="s">
+        <v>4207</v>
+      </c>
+    </row>
+    <row r="558" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B558" s="16" t="s">
+        <v>4170</v>
+      </c>
+      <c r="C558" s="16" t="s">
+        <v>4208</v>
+      </c>
+      <c r="D558" t="s">
+        <v>4209</v>
+      </c>
+    </row>
+    <row r="559" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B559" s="16" t="s">
+        <v>4170</v>
+      </c>
+      <c r="C559" s="16" t="s">
+        <v>4211</v>
+      </c>
+      <c r="D559" t="s">
+        <v>4210</v>
+      </c>
+    </row>
+    <row r="560" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B560" s="16" t="s">
+        <v>4171</v>
+      </c>
+      <c r="C560" s="16" t="s">
+        <v>4212</v>
+      </c>
+      <c r="D560" t="s">
+        <v>4213</v>
+      </c>
+    </row>
+    <row r="561" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B561" s="16" t="s">
+        <v>4171</v>
+      </c>
+      <c r="C561" s="16" t="s">
+        <v>4214</v>
+      </c>
+      <c r="D561" t="s">
+        <v>4215</v>
+      </c>
+    </row>
+    <row r="562" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B562" s="16" t="s">
+        <v>4171</v>
+      </c>
+      <c r="C562" s="16" t="s">
+        <v>4217</v>
+      </c>
+      <c r="D562" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="563" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B563" s="16" t="s">
+        <v>4171</v>
+      </c>
+      <c r="C563" s="16" t="s">
+        <v>4219</v>
+      </c>
+      <c r="D563" t="s">
+        <v>4218</v>
+      </c>
+    </row>
+    <row r="564" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B564" s="16" t="s">
+        <v>4172</v>
+      </c>
+      <c r="C564" s="16" t="s">
+        <v>4220</v>
+      </c>
+      <c r="D564" t="s">
+        <v>4221</v>
+      </c>
+    </row>
+    <row r="565" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B565" s="16" t="s">
+        <v>4172</v>
+      </c>
+      <c r="C565" s="16" t="s">
+        <v>4222</v>
+      </c>
+      <c r="D565" t="s">
+        <v>4223</v>
+      </c>
+    </row>
+    <row r="566" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B566" s="16" t="s">
+        <v>4172</v>
+      </c>
+      <c r="C566" s="16" t="s">
+        <v>4225</v>
+      </c>
+      <c r="D566" t="s">
+        <v>4224</v>
+      </c>
+    </row>
+    <row r="567" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B567" s="16" t="s">
+        <v>4173</v>
+      </c>
+      <c r="C567" s="16" t="s">
+        <v>4226</v>
+      </c>
+      <c r="D567" t="s">
+        <v>4190</v>
+      </c>
+    </row>
+    <row r="568" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B568" s="16" t="s">
+        <v>4174</v>
+      </c>
+      <c r="C568" s="16" t="s">
+        <v>4229</v>
+      </c>
+      <c r="D568" t="s">
+        <v>4227</v>
+      </c>
+    </row>
+    <row r="569" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B569" s="16" t="s">
+        <v>4174</v>
+      </c>
+      <c r="C569" s="16" t="s">
+        <v>4230</v>
+      </c>
+      <c r="D569" t="s">
+        <v>4228</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:Z536">
     <sortCondition ref="A2:A536"/>

</xml_diff>

<commit_message>
Added the Big Hike
</commit_message>
<xml_diff>
--- a/Data/Trail Mapping Info.xlsx
+++ b/Data/Trail Mapping Info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tracks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12132" uniqueCount="4231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12294" uniqueCount="4294">
   <si>
     <t>trackID</t>
   </si>
@@ -12714,6 +12714,195 @@
   </si>
   <si>
     <t>IMG_5174</t>
+  </si>
+  <si>
+    <t>POCL01</t>
+  </si>
+  <si>
+    <t>POCL02</t>
+  </si>
+  <si>
+    <t>POCL03</t>
+  </si>
+  <si>
+    <t>POCL04</t>
+  </si>
+  <si>
+    <t>POCL05</t>
+  </si>
+  <si>
+    <t>POCL06</t>
+  </si>
+  <si>
+    <t>POCL07</t>
+  </si>
+  <si>
+    <t>POCL08</t>
+  </si>
+  <si>
+    <t>POCL09</t>
+  </si>
+  <si>
+    <t>POCL10</t>
+  </si>
+  <si>
+    <t>Fremont Saddle</t>
+  </si>
+  <si>
+    <t>Weaver's Needle Tr</t>
+  </si>
+  <si>
+    <t>leave Peralta Tr</t>
+  </si>
+  <si>
+    <t>Peralta to Canyon Lake Hike (Dutchman's Tr 104)</t>
+  </si>
+  <si>
+    <t>Bull Pass Tr (129)</t>
+  </si>
+  <si>
+    <t>start Dutchman's Tr</t>
+  </si>
+  <si>
+    <t>start Boulder Canyon Tr</t>
+  </si>
+  <si>
+    <t>Cavalry Tr (239)</t>
+  </si>
+  <si>
+    <t>Peralta to Canyon Lake Hike (Boulder Canyon Tr 103)</t>
+  </si>
+  <si>
+    <t>leave Boulder Canyon Tr</t>
+  </si>
+  <si>
+    <t>start Boulder Canyon Tr ALT</t>
+  </si>
+  <si>
+    <t>leave Boulder Canyon Tr ALT</t>
+  </si>
+  <si>
+    <t>arrive Canyon Lake Marina</t>
+  </si>
+  <si>
+    <t>Peralta to Canyon Lake Hike (Boulder Canyon Tr ALT)</t>
+  </si>
+  <si>
+    <t>Peralta to Canyon Lake Hike (Peralta Tr 102)</t>
+  </si>
+  <si>
+    <t>IMG_4975</t>
+  </si>
+  <si>
+    <t>Taking off!</t>
+  </si>
+  <si>
+    <t>IMG_4977</t>
+  </si>
+  <si>
+    <t>IMG_4978</t>
+  </si>
+  <si>
+    <t>IMG_4981</t>
+  </si>
+  <si>
+    <t>First sight of water for the day</t>
+  </si>
+  <si>
+    <t>IMG_4983</t>
+  </si>
+  <si>
+    <t>IMG_4985</t>
+  </si>
+  <si>
+    <t>IMG_4989</t>
+  </si>
+  <si>
+    <t>IMG_4993</t>
+  </si>
+  <si>
+    <t>IMG_4999</t>
+  </si>
+  <si>
+    <t>IMG_5002</t>
+  </si>
+  <si>
+    <t>IMG_5005</t>
+  </si>
+  <si>
+    <t>IMG_5007</t>
+  </si>
+  <si>
+    <t>Looking back to Weaver's Needle</t>
+  </si>
+  <si>
+    <t>IMG_5009</t>
+  </si>
+  <si>
+    <t>IMG_5011</t>
+  </si>
+  <si>
+    <t>IMG_5016</t>
+  </si>
+  <si>
+    <t>IMG_5017</t>
+  </si>
+  <si>
+    <t>Looking north down Boulder Canyon</t>
+  </si>
+  <si>
+    <t>IMG_5020</t>
+  </si>
+  <si>
+    <t>Kim crossing the stream</t>
+  </si>
+  <si>
+    <t>IMG_5023</t>
+  </si>
+  <si>
+    <t>IMG_5024</t>
+  </si>
+  <si>
+    <t>IMG_5027</t>
+  </si>
+  <si>
+    <t>IMG_5030</t>
+  </si>
+  <si>
+    <t>IMG_5032</t>
+  </si>
+  <si>
+    <t>IMG_5040</t>
+  </si>
+  <si>
+    <t>First view of Canyon Lake</t>
+  </si>
+  <si>
+    <t>IMG_5045</t>
+  </si>
+  <si>
+    <t>IMG_5046</t>
+  </si>
+  <si>
+    <t>One last look at Weaver's Needle</t>
+  </si>
+  <si>
+    <t>IMG_5051</t>
+  </si>
+  <si>
+    <t>Canyon Lake (and marina)</t>
+  </si>
+  <si>
+    <t>IMG_5053</t>
+  </si>
+  <si>
+    <t>We made it!</t>
+  </si>
+  <si>
+    <t>Our Support Team</t>
+  </si>
+  <si>
+    <t>IMG_5056</t>
   </si>
 </sst>
 </file>
@@ -13062,20 +13251,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X1200"/>
+  <dimension ref="A1:X1209"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1170" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B1197" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1187" sqref="D1187:D1199"/>
+      <selection pane="bottomRight" activeCell="C1203" sqref="C1203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.21875" bestFit="1" customWidth="1"/>
@@ -45589,7 +45778,289 @@
       </c>
     </row>
     <row r="1200" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1200" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1200" s="3" t="s">
+        <v>4231</v>
+      </c>
+      <c r="C1200" s="3" t="s">
+        <v>4255</v>
+      </c>
+      <c r="D1200">
+        <v>2023</v>
+      </c>
+      <c r="E1200" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1200" s="3" t="s">
+        <v>4080</v>
+      </c>
+      <c r="G1200" s="3" t="s">
+        <v>4241</v>
+      </c>
       <c r="H1200" s="3"/>
+      <c r="I1200" s="3" t="s">
+        <v>4232</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1201" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1201" s="3" t="s">
+        <v>4232</v>
+      </c>
+      <c r="C1201" s="3" t="s">
+        <v>4255</v>
+      </c>
+      <c r="D1201">
+        <v>2023</v>
+      </c>
+      <c r="E1201" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1201" s="3" t="s">
+        <v>4241</v>
+      </c>
+      <c r="G1201" s="3" t="s">
+        <v>4242</v>
+      </c>
+      <c r="H1201" s="3" t="s">
+        <v>4231</v>
+      </c>
+      <c r="I1201" s="3" t="s">
+        <v>4233</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1202" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1202" s="3" t="s">
+        <v>4233</v>
+      </c>
+      <c r="C1202" s="3" t="s">
+        <v>4255</v>
+      </c>
+      <c r="D1202">
+        <v>2023</v>
+      </c>
+      <c r="E1202" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1202" s="3" t="s">
+        <v>4242</v>
+      </c>
+      <c r="G1202" s="3" t="s">
+        <v>4243</v>
+      </c>
+      <c r="H1202" s="3" t="s">
+        <v>4232</v>
+      </c>
+      <c r="I1202" s="3" t="s">
+        <v>4234</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1203" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1203" s="3" t="s">
+        <v>4234</v>
+      </c>
+      <c r="C1203" s="3" t="s">
+        <v>4244</v>
+      </c>
+      <c r="D1203">
+        <v>2023</v>
+      </c>
+      <c r="E1203" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1203" s="3" t="s">
+        <v>4246</v>
+      </c>
+      <c r="G1203" s="3" t="s">
+        <v>4245</v>
+      </c>
+      <c r="H1203" s="3" t="s">
+        <v>4233</v>
+      </c>
+      <c r="I1203" s="3" t="s">
+        <v>4235</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1204" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1204" s="3" t="s">
+        <v>4235</v>
+      </c>
+      <c r="C1204" s="3" t="s">
+        <v>4244</v>
+      </c>
+      <c r="D1204">
+        <v>2023</v>
+      </c>
+      <c r="E1204" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1204" s="3" t="s">
+        <v>4245</v>
+      </c>
+      <c r="G1204" s="3" t="s">
+        <v>4126</v>
+      </c>
+      <c r="H1204" s="3" t="s">
+        <v>4234</v>
+      </c>
+      <c r="I1204" s="3" t="s">
+        <v>4236</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1205" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1205" s="3" t="s">
+        <v>4236</v>
+      </c>
+      <c r="C1205" s="3" t="s">
+        <v>4249</v>
+      </c>
+      <c r="D1205">
+        <v>2023</v>
+      </c>
+      <c r="E1205" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1205" s="3" t="s">
+        <v>4247</v>
+      </c>
+      <c r="G1205" s="3" t="s">
+        <v>4248</v>
+      </c>
+      <c r="H1205" s="3" t="s">
+        <v>4235</v>
+      </c>
+      <c r="I1205" s="3" t="s">
+        <v>4237</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1206" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1206" s="3" t="s">
+        <v>4237</v>
+      </c>
+      <c r="C1206" s="3" t="s">
+        <v>4249</v>
+      </c>
+      <c r="D1206">
+        <v>2023</v>
+      </c>
+      <c r="E1206" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1206" s="3" t="s">
+        <v>4248</v>
+      </c>
+      <c r="G1206" s="3" t="s">
+        <v>3509</v>
+      </c>
+      <c r="H1206" s="3" t="s">
+        <v>4236</v>
+      </c>
+      <c r="I1206" s="3" t="s">
+        <v>4238</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1207" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1207" s="3" t="s">
+        <v>4238</v>
+      </c>
+      <c r="C1207" s="3" t="s">
+        <v>4249</v>
+      </c>
+      <c r="D1207">
+        <v>2023</v>
+      </c>
+      <c r="E1207" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1207" s="3" t="s">
+        <v>3509</v>
+      </c>
+      <c r="G1207" s="3" t="s">
+        <v>4250</v>
+      </c>
+      <c r="H1207" s="3" t="s">
+        <v>4237</v>
+      </c>
+      <c r="I1207" s="3" t="s">
+        <v>4239</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1208" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1208" s="3" t="s">
+        <v>4239</v>
+      </c>
+      <c r="C1208" s="3" t="s">
+        <v>4254</v>
+      </c>
+      <c r="D1208">
+        <v>2023</v>
+      </c>
+      <c r="E1208" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1208" s="3" t="s">
+        <v>4251</v>
+      </c>
+      <c r="G1208" s="3" t="s">
+        <v>4252</v>
+      </c>
+      <c r="H1208" s="3" t="s">
+        <v>4238</v>
+      </c>
+      <c r="I1208" s="3" t="s">
+        <v>4240</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1209" s="3" t="s">
+        <v>3485</v>
+      </c>
+      <c r="B1209" s="3" t="s">
+        <v>4240</v>
+      </c>
+      <c r="C1209" s="3" t="s">
+        <v>4249</v>
+      </c>
+      <c r="D1209">
+        <v>2023</v>
+      </c>
+      <c r="E1209" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1209" s="3" t="s">
+        <v>4247</v>
+      </c>
+      <c r="G1209" s="3" t="s">
+        <v>4253</v>
+      </c>
+      <c r="H1209" s="3" t="s">
+        <v>4239</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:X1186">
@@ -71927,11 +72398,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z569"/>
+  <dimension ref="A1:Y597"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A547" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C570" sqref="C570"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A575" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C598" sqref="C598"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -71942,7 +72413,7 @@
     <col min="4" max="4" width="41.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -71976,9 +72447,8 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>3664</v>
       </c>
@@ -71992,7 +72462,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72006,7 +72476,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72020,7 +72490,7 @@
         <v>3719</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72034,7 +72504,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72048,7 +72518,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72062,7 +72532,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72076,7 +72546,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72090,7 +72560,7 @@
         <v>3779</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72104,7 +72574,7 @@
         <v>3692</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72118,7 +72588,7 @@
         <v>3694</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72132,7 +72602,7 @@
         <v>3693</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72146,7 +72616,7 @@
         <v>3695</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72160,7 +72630,7 @@
         <v>3696</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>3664</v>
       </c>
@@ -72174,7 +72644,7 @@
         <v>3769</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>3664</v>
       </c>
@@ -79839,6 +80309,314 @@
       </c>
       <c r="D569" t="s">
         <v>4228</v>
+      </c>
+    </row>
+    <row r="570" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B570" s="16" t="s">
+        <v>4231</v>
+      </c>
+      <c r="C570" s="16" t="s">
+        <v>4256</v>
+      </c>
+      <c r="D570" t="s">
+        <v>4257</v>
+      </c>
+    </row>
+    <row r="571" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B571" s="16" t="s">
+        <v>4231</v>
+      </c>
+      <c r="C571" s="16" t="s">
+        <v>4258</v>
+      </c>
+      <c r="D571" t="s">
+        <v>4227</v>
+      </c>
+    </row>
+    <row r="572" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B572" s="16" t="s">
+        <v>4231</v>
+      </c>
+      <c r="C572" s="16" t="s">
+        <v>4259</v>
+      </c>
+      <c r="D572" t="s">
+        <v>4228</v>
+      </c>
+    </row>
+    <row r="573" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B573" s="16" t="s">
+        <v>4232</v>
+      </c>
+      <c r="C573" s="16" t="s">
+        <v>4260</v>
+      </c>
+      <c r="D573" t="s">
+        <v>4261</v>
+      </c>
+    </row>
+    <row r="574" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B574" s="16" t="s">
+        <v>4232</v>
+      </c>
+      <c r="C574" s="16" t="s">
+        <v>4262</v>
+      </c>
+      <c r="D574" t="s">
+        <v>4275</v>
+      </c>
+    </row>
+    <row r="575" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B575" s="16" t="s">
+        <v>4233</v>
+      </c>
+      <c r="C575" s="16" t="s">
+        <v>4263</v>
+      </c>
+      <c r="D575" t="s">
+        <v>4270</v>
+      </c>
+    </row>
+    <row r="576" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B576" s="16" t="s">
+        <v>4233</v>
+      </c>
+      <c r="C576" s="16" t="s">
+        <v>4264</v>
+      </c>
+      <c r="D576" t="s">
+        <v>3714</v>
+      </c>
+    </row>
+    <row r="577" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B577" s="16" t="s">
+        <v>4233</v>
+      </c>
+      <c r="C577" s="16" t="s">
+        <v>4265</v>
+      </c>
+      <c r="D577" t="s">
+        <v>3652</v>
+      </c>
+    </row>
+    <row r="578" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B578" s="16" t="s">
+        <v>4233</v>
+      </c>
+      <c r="C578" s="16" t="s">
+        <v>4266</v>
+      </c>
+      <c r="D578" t="s">
+        <v>4270</v>
+      </c>
+    </row>
+    <row r="579" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B579" s="16" t="s">
+        <v>4233</v>
+      </c>
+      <c r="C579" s="16" t="s">
+        <v>4267</v>
+      </c>
+      <c r="D579" t="s">
+        <v>4270</v>
+      </c>
+    </row>
+    <row r="580" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B580" s="16" t="s">
+        <v>4233</v>
+      </c>
+      <c r="C580" s="16" t="s">
+        <v>4268</v>
+      </c>
+      <c r="D580" t="s">
+        <v>4270</v>
+      </c>
+    </row>
+    <row r="581" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B581" s="16" t="s">
+        <v>4234</v>
+      </c>
+      <c r="C581" s="16" t="s">
+        <v>4269</v>
+      </c>
+      <c r="D581" t="s">
+        <v>4270</v>
+      </c>
+    </row>
+    <row r="582" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B582" s="16" t="s">
+        <v>4234</v>
+      </c>
+      <c r="C582" s="16" t="s">
+        <v>4271</v>
+      </c>
+      <c r="D582" t="s">
+        <v>3714</v>
+      </c>
+    </row>
+    <row r="583" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B583" s="16" t="s">
+        <v>4234</v>
+      </c>
+      <c r="C583" s="16" t="s">
+        <v>4272</v>
+      </c>
+      <c r="D583" t="s">
+        <v>4270</v>
+      </c>
+    </row>
+    <row r="584" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B584" s="16" t="s">
+        <v>4236</v>
+      </c>
+      <c r="C584" s="16" t="s">
+        <v>4273</v>
+      </c>
+      <c r="D584" t="s">
+        <v>4270</v>
+      </c>
+    </row>
+    <row r="585" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B585" s="16" t="s">
+        <v>4236</v>
+      </c>
+      <c r="C585" s="16" t="s">
+        <v>4274</v>
+      </c>
+      <c r="D585" t="s">
+        <v>4275</v>
+      </c>
+    </row>
+    <row r="586" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B586" s="16" t="s">
+        <v>4236</v>
+      </c>
+      <c r="C586" s="16" t="s">
+        <v>4276</v>
+      </c>
+      <c r="D586" t="s">
+        <v>4277</v>
+      </c>
+    </row>
+    <row r="587" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B587" s="16" t="s">
+        <v>4236</v>
+      </c>
+      <c r="C587" s="16" t="s">
+        <v>4278</v>
+      </c>
+      <c r="D587" t="s">
+        <v>3714</v>
+      </c>
+    </row>
+    <row r="588" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B588" s="16" t="s">
+        <v>4236</v>
+      </c>
+      <c r="C588" s="16" t="s">
+        <v>4279</v>
+      </c>
+      <c r="D588" t="s">
+        <v>3714</v>
+      </c>
+    </row>
+    <row r="589" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B589" s="16" t="s">
+        <v>4237</v>
+      </c>
+      <c r="C589" s="16" t="s">
+        <v>4280</v>
+      </c>
+      <c r="D589" t="s">
+        <v>3714</v>
+      </c>
+    </row>
+    <row r="590" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B590" s="16" t="s">
+        <v>4238</v>
+      </c>
+      <c r="C590" s="16" t="s">
+        <v>4281</v>
+      </c>
+      <c r="D590" t="s">
+        <v>3714</v>
+      </c>
+    </row>
+    <row r="591" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B591" s="16" t="s">
+        <v>4238</v>
+      </c>
+      <c r="C591" s="16" t="s">
+        <v>4282</v>
+      </c>
+      <c r="D591" t="s">
+        <v>3714</v>
+      </c>
+    </row>
+    <row r="592" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B592" s="16" t="s">
+        <v>4238</v>
+      </c>
+      <c r="C592" s="16" t="s">
+        <v>4283</v>
+      </c>
+      <c r="D592" t="s">
+        <v>3714</v>
+      </c>
+    </row>
+    <row r="593" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B593" s="16" t="s">
+        <v>4238</v>
+      </c>
+      <c r="C593" s="16" t="s">
+        <v>4285</v>
+      </c>
+      <c r="D593" t="s">
+        <v>4284</v>
+      </c>
+    </row>
+    <row r="594" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B594" s="16" t="s">
+        <v>4238</v>
+      </c>
+      <c r="C594" s="16" t="s">
+        <v>4286</v>
+      </c>
+      <c r="D594" t="s">
+        <v>4287</v>
+      </c>
+    </row>
+    <row r="595" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B595" s="16" t="s">
+        <v>4239</v>
+      </c>
+      <c r="C595" s="16" t="s">
+        <v>4288</v>
+      </c>
+      <c r="D595" t="s">
+        <v>4289</v>
+      </c>
+    </row>
+    <row r="596" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B596" s="16" t="s">
+        <v>4240</v>
+      </c>
+      <c r="C596" s="16" t="s">
+        <v>4290</v>
+      </c>
+      <c r="D596" t="s">
+        <v>4291</v>
+      </c>
+    </row>
+    <row r="597" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B597" s="16" t="s">
+        <v>4240</v>
+      </c>
+      <c r="C597" s="16" t="s">
+        <v>4293</v>
+      </c>
+      <c r="D597" t="s">
+        <v>4292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Boca Negra Canyon
</commit_message>
<xml_diff>
--- a/Data/Trail Mapping Info.xlsx
+++ b/Data/Trail Mapping Info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tracks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12417" uniqueCount="4342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12486" uniqueCount="4372">
   <si>
     <t>trackID</t>
   </si>
@@ -13047,6 +13047,96 @@
   </si>
   <si>
     <t>IMG_0804</t>
+  </si>
+  <si>
+    <t>BNMP01</t>
+  </si>
+  <si>
+    <t>Mesa Point TR in Boca Negra Canyon</t>
+  </si>
+  <si>
+    <t>BNMP02</t>
+  </si>
+  <si>
+    <t>BNMP03</t>
+  </si>
+  <si>
+    <t>BNMP04</t>
+  </si>
+  <si>
+    <t>BNMP05</t>
+  </si>
+  <si>
+    <t>BNMP06</t>
+  </si>
+  <si>
+    <t>Parking lot</t>
+  </si>
+  <si>
+    <t>Lower split in trail</t>
+  </si>
+  <si>
+    <t>Upper split in trail</t>
+  </si>
+  <si>
+    <t>Split for close-up view</t>
+  </si>
+  <si>
+    <t>Peak</t>
+  </si>
+  <si>
+    <t>Close-up view</t>
+  </si>
+  <si>
+    <t>BNMP03, BNMP06</t>
+  </si>
+  <si>
+    <t>BNMP02, BNMP06</t>
+  </si>
+  <si>
+    <t>BNMP04, BNMP05</t>
+  </si>
+  <si>
+    <t>BNMP03, BNMP05</t>
+  </si>
+  <si>
+    <t>BNMP03, BNMP04</t>
+  </si>
+  <si>
+    <t>BNMP01, BNMP02</t>
+  </si>
+  <si>
+    <t>BNMP01, BNMP06</t>
+  </si>
+  <si>
+    <t>BNMP02, BNMP03</t>
+  </si>
+  <si>
+    <t>IMG_4734</t>
+  </si>
+  <si>
+    <t>IMG_4735</t>
+  </si>
+  <si>
+    <t>IMG_4736</t>
+  </si>
+  <si>
+    <t>IMG_4737</t>
+  </si>
+  <si>
+    <t>IMG_4739</t>
+  </si>
+  <si>
+    <t>IMG_4741</t>
+  </si>
+  <si>
+    <t>IMG_4742</t>
+  </si>
+  <si>
+    <t>IMG_4743</t>
+  </si>
+  <si>
+    <t>Petroglyph</t>
   </si>
 </sst>
 </file>
@@ -13395,13 +13485,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X1219"/>
+  <dimension ref="A1:X1225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B1197" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1210" sqref="B1210"/>
+      <selection pane="bottomRight" activeCell="H1226" sqref="H1226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -46489,6 +46579,172 @@
       </c>
       <c r="I1219" s="3" t="s">
         <v>4321</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1220" s="3" t="s">
+        <v>4294</v>
+      </c>
+      <c r="B1220" s="3" t="s">
+        <v>4342</v>
+      </c>
+      <c r="C1220" s="3" t="s">
+        <v>4343</v>
+      </c>
+      <c r="D1220">
+        <v>2023</v>
+      </c>
+      <c r="E1220" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1220" s="3" t="s">
+        <v>4349</v>
+      </c>
+      <c r="G1220" s="3" t="s">
+        <v>4350</v>
+      </c>
+      <c r="I1220" s="3" t="s">
+        <v>4356</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1221" s="3" t="s">
+        <v>4294</v>
+      </c>
+      <c r="B1221" s="3" t="s">
+        <v>4344</v>
+      </c>
+      <c r="C1221" s="3" t="s">
+        <v>4343</v>
+      </c>
+      <c r="D1221">
+        <v>2023</v>
+      </c>
+      <c r="E1221" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1221" s="3" t="s">
+        <v>4350</v>
+      </c>
+      <c r="G1221" s="3" t="s">
+        <v>4351</v>
+      </c>
+      <c r="H1221" s="3" t="s">
+        <v>4361</v>
+      </c>
+      <c r="I1221" s="3" t="s">
+        <v>4355</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1222" s="3" t="s">
+        <v>4294</v>
+      </c>
+      <c r="B1222" s="3" t="s">
+        <v>4345</v>
+      </c>
+      <c r="C1222" s="3" t="s">
+        <v>4343</v>
+      </c>
+      <c r="D1222">
+        <v>2023</v>
+      </c>
+      <c r="E1222" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1222" s="3" t="s">
+        <v>4351</v>
+      </c>
+      <c r="G1222" s="3" t="s">
+        <v>4352</v>
+      </c>
+      <c r="H1222" s="3" t="s">
+        <v>4356</v>
+      </c>
+      <c r="I1222" s="3" t="s">
+        <v>4357</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1223" s="3" t="s">
+        <v>4294</v>
+      </c>
+      <c r="B1223" s="3" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C1223" s="3" t="s">
+        <v>4343</v>
+      </c>
+      <c r="D1223">
+        <v>2023</v>
+      </c>
+      <c r="E1223" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1223" s="3" t="s">
+        <v>4352</v>
+      </c>
+      <c r="G1223" s="3" t="s">
+        <v>4353</v>
+      </c>
+      <c r="H1223" s="3" t="s">
+        <v>4358</v>
+      </c>
+      <c r="I1223" s="3"/>
+    </row>
+    <row r="1224" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1224" s="3" t="s">
+        <v>4294</v>
+      </c>
+      <c r="B1224" s="3" t="s">
+        <v>4347</v>
+      </c>
+      <c r="C1224" s="3" t="s">
+        <v>4343</v>
+      </c>
+      <c r="D1224">
+        <v>2023</v>
+      </c>
+      <c r="E1224" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1224" s="3" t="s">
+        <v>4352</v>
+      </c>
+      <c r="G1224" s="3" t="s">
+        <v>4354</v>
+      </c>
+      <c r="H1224" s="3" t="s">
+        <v>4359</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1225" s="3" t="s">
+        <v>4294</v>
+      </c>
+      <c r="B1225" s="3" t="s">
+        <v>4348</v>
+      </c>
+      <c r="C1225" s="3" t="s">
+        <v>4343</v>
+      </c>
+      <c r="D1225">
+        <v>2023</v>
+      </c>
+      <c r="E1225" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1225" s="3" t="s">
+        <v>4351</v>
+      </c>
+      <c r="G1225" s="3" t="s">
+        <v>4350</v>
+      </c>
+      <c r="H1225" s="3" t="s">
+        <v>4362</v>
+      </c>
+      <c r="I1225" s="3" t="s">
+        <v>4360</v>
       </c>
     </row>
   </sheetData>
@@ -72827,11 +73083,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y612"/>
+  <dimension ref="A1:Y620"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A592" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C602" sqref="C602"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A595" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B622" sqref="B622"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -81213,6 +81469,94 @@
         <v>3714</v>
       </c>
     </row>
+    <row r="613" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B613" t="s">
+        <v>4344</v>
+      </c>
+      <c r="C613" s="16" t="s">
+        <v>4363</v>
+      </c>
+      <c r="D613" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="614" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B614" t="s">
+        <v>4345</v>
+      </c>
+      <c r="C614" s="16" t="s">
+        <v>4364</v>
+      </c>
+      <c r="D614" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="615" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B615" t="s">
+        <v>4345</v>
+      </c>
+      <c r="C615" s="16" t="s">
+        <v>4365</v>
+      </c>
+      <c r="D615" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="616" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B616" t="s">
+        <v>4347</v>
+      </c>
+      <c r="C616" s="16" t="s">
+        <v>4366</v>
+      </c>
+      <c r="D616" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="617" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B617" t="s">
+        <v>4347</v>
+      </c>
+      <c r="C617" s="16" t="s">
+        <v>4367</v>
+      </c>
+      <c r="D617" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="618" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B618" t="s">
+        <v>4347</v>
+      </c>
+      <c r="C618" s="16" t="s">
+        <v>4368</v>
+      </c>
+      <c r="D618" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="619" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B619" t="s">
+        <v>4348</v>
+      </c>
+      <c r="C619" s="16" t="s">
+        <v>4369</v>
+      </c>
+      <c r="D619" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="620" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B620" t="s">
+        <v>4342</v>
+      </c>
+      <c r="C620" s="16" t="s">
+        <v>4370</v>
+      </c>
+      <c r="D620" t="s">
+        <v>4371</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:Z536">
     <sortCondition ref="A2:A536"/>

</xml_diff>

<commit_message>
Added Piedra Marcadas trail
</commit_message>
<xml_diff>
--- a/Data/Trail Mapping Info.xlsx
+++ b/Data/Trail Mapping Info.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12486" uniqueCount="4372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12556" uniqueCount="4398">
   <si>
     <t>trackID</t>
   </si>
@@ -13137,6 +13137,84 @@
   </si>
   <si>
     <t>Petroglyph</t>
+  </si>
+  <si>
+    <t>PDMC01</t>
+  </si>
+  <si>
+    <t>PDMC02</t>
+  </si>
+  <si>
+    <t>PDMC03</t>
+  </si>
+  <si>
+    <t>PDMC04</t>
+  </si>
+  <si>
+    <t>PDMC09</t>
+  </si>
+  <si>
+    <t>Piedras Marcadas Hike</t>
+  </si>
+  <si>
+    <t>Split in loop trail</t>
+  </si>
+  <si>
+    <t>Split to deadend trail</t>
+  </si>
+  <si>
+    <t>Neighborhood access trail</t>
+  </si>
+  <si>
+    <t>PDMC02, PDMC04</t>
+  </si>
+  <si>
+    <t>PDMC01, PDMC04</t>
+  </si>
+  <si>
+    <t>PDMC03, PDMC09</t>
+  </si>
+  <si>
+    <t>PDMC02, PDMC09</t>
+  </si>
+  <si>
+    <t>PDMC01, PDMC02</t>
+  </si>
+  <si>
+    <t>PDMC02, PDMC03</t>
+  </si>
+  <si>
+    <t>IMG_4744</t>
+  </si>
+  <si>
+    <t>IMG_4746</t>
+  </si>
+  <si>
+    <t>IMG_4752</t>
+  </si>
+  <si>
+    <t>IMG_4755</t>
+  </si>
+  <si>
+    <t>IMG_4757</t>
+  </si>
+  <si>
+    <t>IMG_4759</t>
+  </si>
+  <si>
+    <t>IMG_4760</t>
+  </si>
+  <si>
+    <t>IMG_4763</t>
+  </si>
+  <si>
+    <t>IMG_4764</t>
+  </si>
+  <si>
+    <t>IMG_4766</t>
+  </si>
+  <si>
+    <t>IMG_4769</t>
   </si>
 </sst>
 </file>
@@ -13485,13 +13563,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X1225"/>
+  <dimension ref="A1:X1230"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1197" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1214" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H1226" sqref="H1226"/>
+      <selection pane="bottomRight" activeCell="B1227" sqref="B1227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -46745,6 +46823,142 @@
       </c>
       <c r="I1225" s="3" t="s">
         <v>4360</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1226" s="3" t="s">
+        <v>4294</v>
+      </c>
+      <c r="B1226" t="s">
+        <v>4372</v>
+      </c>
+      <c r="C1226" t="s">
+        <v>4377</v>
+      </c>
+      <c r="D1226">
+        <v>2023</v>
+      </c>
+      <c r="E1226" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1226" s="3" t="s">
+        <v>4349</v>
+      </c>
+      <c r="G1226" s="3" t="s">
+        <v>4378</v>
+      </c>
+      <c r="I1226" s="3" t="s">
+        <v>4381</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1227" s="3" t="s">
+        <v>4294</v>
+      </c>
+      <c r="B1227" t="s">
+        <v>4373</v>
+      </c>
+      <c r="C1227" t="s">
+        <v>4377</v>
+      </c>
+      <c r="D1227">
+        <v>2023</v>
+      </c>
+      <c r="E1227" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1227" s="3" t="s">
+        <v>4378</v>
+      </c>
+      <c r="G1227" s="3" t="s">
+        <v>4379</v>
+      </c>
+      <c r="H1227" s="3" t="s">
+        <v>4382</v>
+      </c>
+      <c r="I1227" s="3" t="s">
+        <v>4383</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1228" s="3" t="s">
+        <v>4294</v>
+      </c>
+      <c r="B1228" t="s">
+        <v>4374</v>
+      </c>
+      <c r="C1228" t="s">
+        <v>4377</v>
+      </c>
+      <c r="D1228">
+        <v>2023</v>
+      </c>
+      <c r="E1228" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1228" s="3" t="s">
+        <v>4379</v>
+      </c>
+      <c r="G1228" s="3" t="s">
+        <v>4380</v>
+      </c>
+      <c r="H1228" s="3" t="s">
+        <v>4384</v>
+      </c>
+      <c r="I1228" s="3" t="s">
+        <v>4375</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1229" s="3" t="s">
+        <v>4294</v>
+      </c>
+      <c r="B1229" t="s">
+        <v>4375</v>
+      </c>
+      <c r="C1229" t="s">
+        <v>4377</v>
+      </c>
+      <c r="D1229">
+        <v>2023</v>
+      </c>
+      <c r="E1229" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1229" s="3" t="s">
+        <v>4380</v>
+      </c>
+      <c r="G1229" s="3" t="s">
+        <v>4378</v>
+      </c>
+      <c r="H1229" s="3" t="s">
+        <v>4374</v>
+      </c>
+      <c r="I1229" s="3" t="s">
+        <v>4385</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1230" s="3" t="s">
+        <v>4294</v>
+      </c>
+      <c r="B1230" t="s">
+        <v>4376</v>
+      </c>
+      <c r="C1230" t="s">
+        <v>4377</v>
+      </c>
+      <c r="D1230">
+        <v>2023</v>
+      </c>
+      <c r="E1230" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1230" s="3" t="s">
+        <v>4379</v>
+      </c>
+      <c r="H1230" s="3" t="s">
+        <v>4386</v>
       </c>
     </row>
   </sheetData>
@@ -73083,11 +73297,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y620"/>
+  <dimension ref="A1:Y631"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A595" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B622" sqref="B622"/>
+      <pane ySplit="1" topLeftCell="A608" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D634" sqref="D634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -81557,6 +81771,127 @@
         <v>4371</v>
       </c>
     </row>
+    <row r="621" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B621" t="s">
+        <v>4373</v>
+      </c>
+      <c r="C621" s="16" t="s">
+        <v>4387</v>
+      </c>
+      <c r="D621" t="s">
+        <v>3714</v>
+      </c>
+    </row>
+    <row r="622" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B622" t="s">
+        <v>4373</v>
+      </c>
+      <c r="C622" s="16" t="s">
+        <v>4388</v>
+      </c>
+      <c r="D622" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="623" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B623" t="s">
+        <v>4373</v>
+      </c>
+      <c r="C623" s="16" t="s">
+        <v>4389</v>
+      </c>
+      <c r="D623" t="s">
+        <v>3714</v>
+      </c>
+    </row>
+    <row r="624" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B624" t="s">
+        <v>4375</v>
+      </c>
+      <c r="C624" s="16" t="s">
+        <v>4390</v>
+      </c>
+      <c r="D624" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="625" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B625" t="s">
+        <v>4375</v>
+      </c>
+      <c r="C625" s="16" t="s">
+        <v>4391</v>
+      </c>
+      <c r="D625" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="626" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B626" t="s">
+        <v>4375</v>
+      </c>
+      <c r="C626" s="16" t="s">
+        <v>4392</v>
+      </c>
+      <c r="D626" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="627" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B627" t="s">
+        <v>4375</v>
+      </c>
+      <c r="C627" s="16" t="s">
+        <v>4393</v>
+      </c>
+      <c r="D627" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="628" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B628" t="s">
+        <v>4375</v>
+      </c>
+      <c r="C628" s="16" t="s">
+        <v>4394</v>
+      </c>
+      <c r="D628" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="629" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B629" t="s">
+        <v>4375</v>
+      </c>
+      <c r="C629" s="16" t="s">
+        <v>4395</v>
+      </c>
+      <c r="D629" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="630" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B630" t="s">
+        <v>4375</v>
+      </c>
+      <c r="C630" s="16" t="s">
+        <v>4396</v>
+      </c>
+      <c r="D630" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="631" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B631" t="s">
+        <v>4375</v>
+      </c>
+      <c r="C631" s="16" t="s">
+        <v>4397</v>
+      </c>
+      <c r="D631" t="s">
+        <v>4371</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:Z536">
     <sortCondition ref="A2:A536"/>

</xml_diff>